<commit_message>
Se finaliza project de fugas y fraudes
</commit_message>
<xml_diff>
--- a/Malla/Malla.xlsx
+++ b/Malla/Malla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arturo\Documents\trendit\Malla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{36D1AA79-743A-4821-BFFD-181017384FC1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4B2AAE5C-AAC8-4D28-8FF7-A92BBE257611}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CE728E4A-D156-4FB4-96FF-41168B829F56}"/>
   </bookViews>
@@ -337,868 +337,868 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="A6" t="str">
-            <v>33548</v>
+            <v>18220</v>
           </cell>
           <cell r="E6">
-            <v>43869.003472222219</v>
+            <v>43910.003472222219</v>
           </cell>
           <cell r="I6">
-            <v>43869.048090277778</v>
-          </cell>
-          <cell r="N6" t="str">
-            <v>PROOSGMM_oinfo_FYF_01</v>
-          </cell>
-          <cell r="Q6" t="str">
-            <v>Ended OK</v>
+            <v>43910.059444444443</v>
+          </cell>
+          <cell r="M6" t="str">
+            <v>PROOSGMM_oinfo_FYF_05</v>
+          </cell>
+          <cell r="P6" t="str">
+            <v>Ended Not OK</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7" t="str">
-            <v>33544</v>
+            <v>18208</v>
           </cell>
           <cell r="E7">
-            <v>43869.003472222219</v>
+            <v>43910.003472222219</v>
           </cell>
           <cell r="I7">
-            <v>43869.080069444448</v>
-          </cell>
-          <cell r="N7" t="str">
-            <v>PROOSGMM_oinfo_FYF_02</v>
-          </cell>
-          <cell r="Q7" t="str">
-            <v>Ended OK</v>
+            <v>43910.04378472222</v>
+          </cell>
+          <cell r="M7" t="str">
+            <v>PROOSGMM_oinfo_FYF_03</v>
+          </cell>
+          <cell r="P7" t="str">
+            <v>Ended Not OK</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8" t="str">
-            <v>33549</v>
+            <v>18203</v>
           </cell>
           <cell r="E8">
-            <v>43869.003472222219</v>
+            <v>43910.003472222219</v>
           </cell>
           <cell r="I8">
-            <v>43869.094722222224</v>
-          </cell>
-          <cell r="N8" t="str">
-            <v>PROOSGMM_oinfo_FYF_05</v>
-          </cell>
-          <cell r="Q8" t="str">
-            <v>Ended OK</v>
+            <v>43910.041331018518</v>
+          </cell>
+          <cell r="M8" t="str">
+            <v>PROOSGMM_oinfo_FYF_02</v>
+          </cell>
+          <cell r="P8" t="str">
+            <v>Ended Not OK</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9" t="str">
-            <v>33546</v>
+            <v>18202</v>
           </cell>
           <cell r="E9">
-            <v>43869.003472222219</v>
+            <v>43910.003472222219</v>
           </cell>
           <cell r="I9">
-            <v>43869.09746527778</v>
-          </cell>
-          <cell r="N9" t="str">
+            <v>43910.037870370368</v>
+          </cell>
+          <cell r="M9" t="str">
             <v>PROOSGMM_oinfo_FYF_04</v>
           </cell>
-          <cell r="Q9" t="str">
-            <v>Ended OK</v>
+          <cell r="P9" t="str">
+            <v>Ended Not OK</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10" t="str">
-            <v>33547</v>
+            <v>18204</v>
           </cell>
           <cell r="E10">
-            <v>43869.003472222219</v>
+            <v>43910.003472222219</v>
           </cell>
           <cell r="I10">
-            <v>43869.104537037034</v>
-          </cell>
-          <cell r="N10" t="str">
-            <v>PROOSGMM_oinfo_FYF_03</v>
-          </cell>
-          <cell r="Q10" t="str">
-            <v>Ended Not OK</v>
+            <v>43910.027314814812</v>
+          </cell>
+          <cell r="M10" t="str">
+            <v>PROOSGMM_oinfo_FYF_01</v>
+          </cell>
+          <cell r="P10" t="str">
+            <v>Ended OK</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11" t="str">
-            <v>37259</v>
+            <v>23380</v>
           </cell>
           <cell r="E11">
-            <v>43869.006944444445</v>
+            <v>43910.006944444445</v>
           </cell>
           <cell r="I11">
-            <v>43869.106203703705</v>
-          </cell>
-          <cell r="N11" t="str">
+            <v>43910.060833333337</v>
+          </cell>
+          <cell r="M11" t="str">
             <v>PROOSGMM_oinfo_GMM_05</v>
           </cell>
-          <cell r="Q11" t="str">
-            <v>Ended OK</v>
+          <cell r="P11" t="str">
+            <v>Ended Not OK</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12" t="str">
-            <v>11230</v>
+            <v>10164</v>
           </cell>
           <cell r="E12">
-            <v>43869.072916666664</v>
+            <v>43910.072916666664</v>
           </cell>
           <cell r="I12">
-            <v>43869.139166666668</v>
-          </cell>
-          <cell r="N12" t="str">
+            <v>43910.12709490741</v>
+          </cell>
+          <cell r="M12" t="str">
             <v>PROOSGMM_oinfo_GMM_01</v>
           </cell>
-          <cell r="Q12" t="str">
+          <cell r="P12" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13" t="str">
-            <v>23694</v>
+            <v>13695</v>
           </cell>
           <cell r="E13">
-            <v>43869.083333333336</v>
+            <v>43910.083333333336</v>
           </cell>
           <cell r="I13">
-            <v>43869.121215277781</v>
-          </cell>
-          <cell r="N13" t="str">
+            <v>43910.126747685186</v>
+          </cell>
+          <cell r="M13" t="str">
             <v>PROOSGMM_oinfo_GMM_04</v>
           </cell>
-          <cell r="Q13" t="str">
+          <cell r="P13" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14" t="str">
-            <v>41191</v>
+            <v>21712</v>
           </cell>
           <cell r="E14">
-            <v>43869.094722222224</v>
+            <v>43910.097222222219</v>
           </cell>
           <cell r="I14">
-            <v>43869.120358796295</v>
-          </cell>
-          <cell r="N14" t="str">
-            <v>PROOSGMM_CNM_PROVEEDOR_MEDICO</v>
-          </cell>
-          <cell r="Q14" t="str">
+            <v>43910.176840277774</v>
+          </cell>
+          <cell r="M14" t="str">
+            <v>PROOSEOT_extevo_EOT_301</v>
+          </cell>
+          <cell r="P14" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15" t="str">
-            <v>22688</v>
+            <v>21713</v>
           </cell>
           <cell r="E15">
-            <v>43869.097222222219</v>
+            <v>43910.097222222219</v>
           </cell>
           <cell r="I15">
-            <v>43869.140543981484</v>
-          </cell>
-          <cell r="N15" t="str">
+            <v>43910.134965277779</v>
+          </cell>
+          <cell r="M15" t="str">
             <v>PROOSEOT_extevo_EOT_101</v>
           </cell>
-          <cell r="Q15" t="str">
+          <cell r="P15" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16" t="str">
-            <v>22689</v>
+            <v>32367</v>
           </cell>
           <cell r="E16">
-            <v>43869.097222222219</v>
+            <v>43910.111111111109</v>
           </cell>
           <cell r="I16">
-            <v>43869.183831018519</v>
-          </cell>
-          <cell r="N16" t="str">
-            <v>PROOSEOT_extevo_EOT_301</v>
-          </cell>
-          <cell r="Q16" t="str">
+            <v>43910.116712962961</v>
+          </cell>
+          <cell r="M16" t="str">
+            <v>PROOSGMM_oinfo_GMM_06</v>
+          </cell>
+          <cell r="P16" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17" t="str">
-            <v>23706</v>
+            <v>10573</v>
           </cell>
           <cell r="E17">
-            <v>43869.09747685185</v>
+            <v>43910.119444444441</v>
           </cell>
           <cell r="I17">
-            <v>43869.13380787037</v>
-          </cell>
-          <cell r="N17" t="str">
-            <v>PROOSGMM_wkf_gmm_taller_producto</v>
-          </cell>
-          <cell r="Q17" t="str">
+            <v>43910.12228009259</v>
+          </cell>
+          <cell r="M17" t="str">
+            <v>PROOSCRM_wkf_cat_padecimiento_icd9</v>
+          </cell>
+          <cell r="P17" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18" t="str">
-            <v>55825</v>
+            <v>11362</v>
           </cell>
           <cell r="E18">
-            <v>43869.111111111109</v>
+            <v>43910.120138888888</v>
           </cell>
           <cell r="I18">
-            <v>43869.117986111109</v>
-          </cell>
-          <cell r="N18" t="str">
-            <v>PROOSGMM_oinfo_GMM_06</v>
-          </cell>
-          <cell r="Q18" t="str">
+            <v>43910.122974537036</v>
+          </cell>
+          <cell r="M18" t="str">
+            <v>PROOSCRM_wkf_cat_region_corporal</v>
+          </cell>
+          <cell r="P18" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19" t="str">
-            <v>683</v>
+            <v>16705</v>
           </cell>
           <cell r="E19">
-            <v>43869.119444444441</v>
+            <v>43910.125694444447</v>
           </cell>
           <cell r="I19">
-            <v>43869.12228009259</v>
-          </cell>
-          <cell r="N19" t="str">
-            <v>PROOSCRM_wkf_cat_padecimiento_icd9</v>
-          </cell>
-          <cell r="Q19" t="str">
+            <v>43910.128518518519</v>
+          </cell>
+          <cell r="M19" t="str">
+            <v>PROOSCRM_wkf_cat_sistema_origen</v>
+          </cell>
+          <cell r="P19" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20" t="str">
-            <v>7177</v>
+            <v>17357</v>
           </cell>
           <cell r="E20">
-            <v>43869.120138888888</v>
+            <v>43910.126388888886</v>
           </cell>
           <cell r="I20">
-            <v>43869.122974537036</v>
-          </cell>
-          <cell r="N20" t="str">
-            <v>PROOSCRM_wkf_cat_region_corporal</v>
-          </cell>
-          <cell r="Q20" t="str">
+            <v>43910.129212962966</v>
+          </cell>
+          <cell r="M20" t="str">
+            <v>PROOSCRM_wkf_cat_grupo_icd</v>
+          </cell>
+          <cell r="P20" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21" t="str">
-            <v>13711</v>
+            <v>24877</v>
           </cell>
           <cell r="E21">
-            <v>43869.125694444447</v>
+            <v>43910.133634259262</v>
           </cell>
           <cell r="I21">
-            <v>43869.128530092596</v>
-          </cell>
-          <cell r="N21" t="str">
-            <v>PROOSCRM_wkf_cat_sistema_origen</v>
-          </cell>
-          <cell r="Q21" t="str">
+            <v>43910.162974537037</v>
+          </cell>
+          <cell r="M21" t="str">
+            <v>PROOSGMM_wkf_gmm_taller_producto</v>
+          </cell>
+          <cell r="P21" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="22">
           <cell r="A22" t="str">
-            <v>14791</v>
+            <v>26051</v>
           </cell>
           <cell r="E22">
-            <v>43869.126388888886</v>
+            <v>43910.134976851848</v>
           </cell>
           <cell r="I22">
-            <v>43869.129224537035</v>
-          </cell>
-          <cell r="N22" t="str">
-            <v>PROOSCRM_wkf_cat_grupo_icd</v>
-          </cell>
-          <cell r="Q22" t="str">
+            <v>43910.21738425926</v>
+          </cell>
+          <cell r="M22" t="str">
+            <v>PROOSEOT_extevo_EOT_251</v>
+          </cell>
+          <cell r="P22" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23" t="str">
-            <v>22741</v>
+            <v>7795</v>
           </cell>
           <cell r="E23">
-            <v>43869.13380787037</v>
+            <v>43910.145833333336</v>
           </cell>
           <cell r="I23">
-            <v>43869.147835648146</v>
-          </cell>
-          <cell r="N23" t="str">
-            <v>PROOSGMM_CNM_POLIZA</v>
-          </cell>
-          <cell r="Q23" t="str">
+            <v>43910.218969907408</v>
+          </cell>
+          <cell r="M23" t="str">
+            <v>PROOSGMM_oinfo_GMM_02</v>
+          </cell>
+          <cell r="P23" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24" t="str">
-            <v>30508</v>
+            <v>25440</v>
           </cell>
           <cell r="E24">
-            <v>43869.140555555554</v>
+            <v>43910.161111111112</v>
           </cell>
           <cell r="I24">
-            <v>43869.227152777778</v>
-          </cell>
-          <cell r="N24" t="str">
-            <v>PROOSEOT_extevo_EOT_251</v>
-          </cell>
-          <cell r="Q24" t="str">
+            <v>43910.182222222225</v>
+          </cell>
+          <cell r="M24" t="str">
+            <v>PROOSGMM_CNM_PROVEEDOR_MEDICO</v>
+          </cell>
+          <cell r="P24" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25" t="str">
-            <v>13972</v>
+            <v>22383</v>
           </cell>
           <cell r="E25">
-            <v>43869.145833333336</v>
+            <v>43910.162986111114</v>
           </cell>
           <cell r="I25">
-            <v>43869.218854166669</v>
-          </cell>
-          <cell r="N25" t="str">
-            <v>PROOSGMM_oinfo_GMM_02</v>
-          </cell>
-          <cell r="Q25" t="str">
+            <v>43910.179745370369</v>
+          </cell>
+          <cell r="M25" t="str">
+            <v>PROOSGMM_CNM_POLIZA</v>
+          </cell>
+          <cell r="P25" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26" t="str">
-            <v>10111</v>
+            <v>25538</v>
           </cell>
           <cell r="E26">
-            <v>43869.147835648146</v>
+            <v>43910.166666666664</v>
           </cell>
           <cell r="I26">
-            <v>43869.193715277775</v>
-          </cell>
-          <cell r="N26" t="str">
-            <v>PROOSGMM_CNM_ASEG_DATOS_ADICIONALES</v>
-          </cell>
-          <cell r="Q26" t="str">
+            <v>43910.173692129632</v>
+          </cell>
+          <cell r="M26" t="str">
+            <v>PROOSGMM_AZUL_wkf_gccticdc</v>
+          </cell>
+          <cell r="P26" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27" t="str">
-            <v>28289</v>
+            <v>25579</v>
           </cell>
           <cell r="E27">
-            <v>43869.166666666664</v>
+            <v>43910.166666666664</v>
           </cell>
           <cell r="I27">
-            <v>43869.172291666669</v>
-          </cell>
-          <cell r="N27" t="str">
-            <v>PROOSGMM_AZUL_wkf_gfvtcna0</v>
-          </cell>
-          <cell r="Q27" t="str">
+            <v>43910.173692129632</v>
+          </cell>
+          <cell r="M27" t="str">
+            <v>PROOSGMM_AZUL_wkf_gfvtfla0</v>
+          </cell>
+          <cell r="P27" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28" t="str">
-            <v>28288</v>
+            <v>25535</v>
           </cell>
           <cell r="E28">
-            <v>43869.166666666664</v>
+            <v>43910.166666666664</v>
           </cell>
           <cell r="I28">
-            <v>43869.172291666669</v>
-          </cell>
-          <cell r="N28" t="str">
-            <v>PROOSGMM_AZUL_wkf_gfvtfla0</v>
-          </cell>
-          <cell r="Q28" t="str">
+            <v>43910.173692129632</v>
+          </cell>
+          <cell r="M28" t="str">
+            <v>PROOSGMM_AZUL_wkf_gfvtcna0</v>
+          </cell>
+          <cell r="P28" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29" t="str">
-            <v>28290</v>
+            <v>25537</v>
           </cell>
           <cell r="E29">
-            <v>43869.166666666664</v>
+            <v>43910.166666666664</v>
           </cell>
           <cell r="I29">
-            <v>43869.172291666669</v>
-          </cell>
-          <cell r="N29" t="str">
-            <v>PROOSGMM_AZUL_wkf_gccticdc</v>
-          </cell>
-          <cell r="Q29" t="str">
+            <v>43910.173692129632</v>
+          </cell>
+          <cell r="M29" t="str">
+            <v>PROOSGMM_AZUL_wkf_gfvtagt0</v>
+          </cell>
+          <cell r="P29" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30" t="str">
-            <v>28283</v>
+            <v>10837</v>
           </cell>
           <cell r="E30">
-            <v>43869.166666666664</v>
+            <v>43910.176851851851</v>
           </cell>
           <cell r="I30">
-            <v>43869.173692129632</v>
-          </cell>
-          <cell r="N30" t="str">
-            <v>PROOSGMM_AZUL_wkf_gfvtagt0</v>
-          </cell>
-          <cell r="Q30" t="str">
+            <v>43910.266215277778</v>
+          </cell>
+          <cell r="M30" t="str">
+            <v>PROOSEOT_extevo_EOT_351</v>
+          </cell>
+          <cell r="P30" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31" t="str">
-            <v>16982</v>
+            <v>17690</v>
           </cell>
           <cell r="E31">
-            <v>43869.183842592596</v>
+            <v>43910.179756944446</v>
           </cell>
           <cell r="I31">
-            <v>43869.270416666666</v>
-          </cell>
-          <cell r="N31" t="str">
-            <v>PROOSEOT_extevo_EOT_351</v>
-          </cell>
-          <cell r="Q31" t="str">
+            <v>43910.225752314815</v>
+          </cell>
+          <cell r="M31" t="str">
+            <v>PROOSGMM_CNM_ASEG_DATOS_ADICIONALES</v>
+          </cell>
+          <cell r="P31" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32" t="str">
-            <v>41190</v>
+            <v>51878</v>
           </cell>
           <cell r="E32">
-            <v>43869.1875</v>
+            <v>43910.1875</v>
           </cell>
           <cell r="I32">
-            <v>43869.190081018518</v>
-          </cell>
-          <cell r="N32" t="str">
+            <v>43910.190925925926</v>
+          </cell>
+          <cell r="M32" t="str">
             <v>PROOSGMM_BDM_valida_recla</v>
           </cell>
-          <cell r="Q32" t="str">
+          <cell r="P32" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="33">
           <cell r="A33" t="str">
-            <v>44852</v>
+            <v>1213</v>
           </cell>
           <cell r="E33">
-            <v>43869.190092592595</v>
+            <v>43910.190937500003</v>
           </cell>
           <cell r="I33">
-            <v>43869.207175925927</v>
-          </cell>
-          <cell r="N33" t="str">
-            <v>PROOSGMM_recla_LMP_NRLTRCL0</v>
-          </cell>
-          <cell r="Q33" t="str">
+            <v>43910.237337962964</v>
+          </cell>
+          <cell r="M33" t="str">
+            <v>PROOSGMM_recla_LMP_NRLTSLR0</v>
+          </cell>
+          <cell r="P33" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="34">
           <cell r="A34" t="str">
-            <v>44858</v>
+            <v>1214</v>
           </cell>
           <cell r="E34">
-            <v>43869.190092592595</v>
+            <v>43910.190937500003</v>
           </cell>
           <cell r="I34">
-            <v>43869.211759259262</v>
-          </cell>
-          <cell r="N34" t="str">
-            <v>PROOSGMM_recla_LMP_NRLTDDC0</v>
-          </cell>
-          <cell r="Q34" t="str">
+            <v>43910.231736111113</v>
+          </cell>
+          <cell r="M34" t="str">
+            <v>PROOSGMM_recla_LMP_NRLTASP0</v>
+          </cell>
+          <cell r="P34" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="35">
           <cell r="A35" t="str">
-            <v>44867</v>
+            <v>1222</v>
           </cell>
           <cell r="E35">
-            <v>43869.190092592595</v>
+            <v>43910.190937500003</v>
           </cell>
           <cell r="I35">
-            <v>43869.21638888889</v>
-          </cell>
-          <cell r="N35" t="str">
+            <v>43910.219398148147</v>
+          </cell>
+          <cell r="M35" t="str">
             <v>PROOSGMM_recla_LMP_NRLTAAN0</v>
           </cell>
-          <cell r="Q35" t="str">
+          <cell r="P35" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="36">
           <cell r="A36" t="str">
-            <v>44851</v>
+            <v>1218</v>
           </cell>
           <cell r="E36">
-            <v>43869.190092592595</v>
+            <v>43910.190937500003</v>
           </cell>
           <cell r="I36">
-            <v>43869.232615740744</v>
-          </cell>
-          <cell r="N36" t="str">
-            <v>PROOSGMM_recla_LMP_NRLTASP0</v>
-          </cell>
-          <cell r="Q36" t="str">
+            <v>43910.212361111109</v>
+          </cell>
+          <cell r="M36" t="str">
+            <v>PROOSGMM_recla_LMP_NRLTRCL0</v>
+          </cell>
+          <cell r="P36" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="37">
           <cell r="A37" t="str">
-            <v>44856</v>
+            <v>1212</v>
           </cell>
           <cell r="E37">
-            <v>43869.190092592595</v>
+            <v>43910.190937500003</v>
           </cell>
           <cell r="I37">
-            <v>43869.232743055552</v>
-          </cell>
-          <cell r="N37" t="str">
-            <v>PROOSGMM_recla_LMP_NRLTSLR0</v>
-          </cell>
-          <cell r="Q37" t="str">
+            <v>43910.212384259263</v>
+          </cell>
+          <cell r="M37" t="str">
+            <v>PROOSGMM_recla_LMP_NRLTCMP0</v>
+          </cell>
+          <cell r="P37" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="38">
           <cell r="A38" t="str">
-            <v>44855</v>
+            <v>1217</v>
           </cell>
           <cell r="E38">
-            <v>43869.190092592595</v>
+            <v>43910.190937500003</v>
           </cell>
           <cell r="I38">
-            <v>43869.245648148149</v>
-          </cell>
-          <cell r="N38" t="str">
-            <v>PROOSGMM_recla_LMP_NRLTCMP0</v>
-          </cell>
-          <cell r="Q38" t="str">
-            <v>Ended OK</v>
+            <v>43910.195717592593</v>
+          </cell>
+          <cell r="M38" t="str">
+            <v>PROOSGMM_recla_LMP_NRLTDDC0</v>
+          </cell>
+          <cell r="P38" t="str">
+            <v>Ended Not OK</v>
           </cell>
         </row>
         <row r="39">
           <cell r="A39" t="str">
-            <v>1435</v>
+            <v>18899</v>
           </cell>
           <cell r="E39">
-            <v>43869.193726851852</v>
+            <v>43910.225763888891</v>
           </cell>
           <cell r="I39">
-            <v>43869.23165509259</v>
-          </cell>
-          <cell r="N39" t="str">
+            <v>43910.272037037037</v>
+          </cell>
+          <cell r="M39" t="str">
             <v>PROOSGMM_CNM_COBERT_DATOS_ADICIONALES</v>
           </cell>
-          <cell r="Q39" t="str">
+          <cell r="P39" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="40">
           <cell r="A40" t="str">
-            <v>2070</v>
+            <v>28882</v>
           </cell>
           <cell r="E40">
-            <v>43869.231666666667</v>
+            <v>43910.231747685182</v>
           </cell>
           <cell r="I40">
-            <v>43869.248240740744</v>
-          </cell>
-          <cell r="N40" t="str">
-            <v>PROOSGMM_CNM_POLIZA_DATOS_ADICIONALES</v>
-          </cell>
-          <cell r="Q40" t="str">
+            <v>43910.248495370368</v>
+          </cell>
+          <cell r="M40" t="str">
+            <v>PROOSGMM_CNM_RECLAMACION</v>
+          </cell>
+          <cell r="P40" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="41">
           <cell r="A41" t="str">
-            <v>2653</v>
+            <v>31926</v>
           </cell>
           <cell r="E41">
-            <v>43869.232615740744</v>
+            <v>43910.232638888891</v>
           </cell>
           <cell r="I41">
-            <v>43869.242407407408</v>
-          </cell>
-          <cell r="N41" t="str">
-            <v>PROOSGMM_CNM_RECLAMACION</v>
-          </cell>
-          <cell r="Q41" t="str">
+            <v>43910.275277777779</v>
+          </cell>
+          <cell r="M41" t="str">
+            <v>PROOSGMM_orecla_LMP</v>
+          </cell>
+          <cell r="P41" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="42">
           <cell r="A42" t="str">
-            <v>24197</v>
+            <v>39835</v>
           </cell>
           <cell r="E42">
-            <v>43869.245659722219</v>
+            <v>43910.237349537034</v>
           </cell>
           <cell r="I42">
-            <v>43869.261770833335</v>
-          </cell>
-          <cell r="N42" t="str">
-            <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_GC</v>
-          </cell>
-          <cell r="Q42" t="str">
+            <v>43910.318437499998</v>
+          </cell>
+          <cell r="M42" t="str">
+            <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_DG</v>
+          </cell>
+          <cell r="P42" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="43">
           <cell r="A43" t="str">
-            <v>24187</v>
+            <v>39839</v>
           </cell>
           <cell r="E43">
-            <v>43869.245659722219</v>
+            <v>43910.237349537034</v>
           </cell>
           <cell r="I43">
-            <v>43869.272488425922</v>
-          </cell>
-          <cell r="N43" t="str">
-            <v>PROOSGMM_orecla_LMP</v>
-          </cell>
-          <cell r="Q43" t="str">
+            <v>43910.288587962961</v>
+          </cell>
+          <cell r="M43" t="str">
+            <v>PROOSGMM_ENR_SOLICITUD</v>
+          </cell>
+          <cell r="P43" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="44">
           <cell r="A44" t="str">
-            <v>24188</v>
+            <v>39838</v>
           </cell>
           <cell r="E44">
-            <v>43869.245659722219</v>
+            <v>43910.237349537034</v>
           </cell>
           <cell r="I44">
-            <v>43869.282430555555</v>
-          </cell>
-          <cell r="N44" t="str">
+            <v>43910.278726851851</v>
+          </cell>
+          <cell r="M44" t="str">
             <v>PROOSGMM_ENR_SOLICITUD_DG</v>
           </cell>
-          <cell r="Q44" t="str">
+          <cell r="P44" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="45">
           <cell r="A45" t="str">
-            <v>24186</v>
+            <v>39834</v>
           </cell>
           <cell r="E45">
-            <v>43869.245659722219</v>
+            <v>43910.237349537034</v>
           </cell>
           <cell r="I45">
-            <v>43869.290543981479</v>
-          </cell>
-          <cell r="N45" t="str">
-            <v>PROOSGMM_ENR_SOLICITUD</v>
-          </cell>
-          <cell r="Q45" t="str">
+            <v>43910.256076388891</v>
+          </cell>
+          <cell r="M45" t="str">
+            <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_GC</v>
+          </cell>
+          <cell r="P45" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46" t="str">
-            <v>24192</v>
+            <v>1923</v>
           </cell>
           <cell r="E46">
-            <v>43869.245659722219</v>
+            <v>43910.263888888891</v>
           </cell>
           <cell r="I46">
-            <v>43869.320798611108</v>
-          </cell>
-          <cell r="N46" t="str">
-            <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_DG</v>
-          </cell>
-          <cell r="Q46" t="str">
+            <v>43910.329768518517</v>
+          </cell>
+          <cell r="M46" t="str">
+            <v>PROOSGMM_oinfo_GMM_03</v>
+          </cell>
+          <cell r="P46" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="47">
           <cell r="A47" t="str">
-            <v>45415</v>
+            <v>29026</v>
           </cell>
           <cell r="E47">
-            <v>43869.263888888891</v>
+            <v>43910.272037037037</v>
           </cell>
           <cell r="I47">
-            <v>43869.322800925926</v>
-          </cell>
-          <cell r="N47" t="str">
-            <v>PROOSGMM_oinfo_GMM_03</v>
-          </cell>
-          <cell r="Q47" t="str">
+            <v>43910.294178240743</v>
+          </cell>
+          <cell r="M47" t="str">
+            <v>PROOSGMM_CNM_POLIZA_DATOS_ADICIONALES</v>
+          </cell>
+          <cell r="P47" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="48">
           <cell r="A48" t="str">
-            <v>9507</v>
+            <v>31171</v>
           </cell>
           <cell r="E48">
-            <v>43869.272499999999</v>
+            <v>43910.275277777779</v>
           </cell>
           <cell r="I48">
-            <v>43869.296967592592</v>
-          </cell>
-          <cell r="N48" t="str">
+            <v>43910.297407407408</v>
+          </cell>
+          <cell r="M48" t="str">
             <v>PROOSGMM_CNM_RECLAMACION_ACUMULADO</v>
           </cell>
-          <cell r="Q48" t="str">
+          <cell r="P48" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="49">
           <cell r="A49" t="str">
-            <v>53006</v>
+            <v>8254</v>
           </cell>
           <cell r="E49">
-            <v>43869.28125</v>
+            <v>43910.28125</v>
           </cell>
           <cell r="I49">
-            <v>43869.288506944446</v>
-          </cell>
-          <cell r="N49" t="str">
+            <v>43910.287557870368</v>
+          </cell>
+          <cell r="M49" t="str">
             <v>PROOSGMM_orecla_01</v>
           </cell>
-          <cell r="Q49" t="str">
+          <cell r="P49" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="50">
           <cell r="A50" t="str">
-            <v>32105</v>
+            <v>25039</v>
           </cell>
           <cell r="E50">
-            <v>43869.288506944446</v>
+            <v>43910.287557870368</v>
           </cell>
           <cell r="I50">
-            <v>43869.3125</v>
-          </cell>
-          <cell r="N50" t="str">
+            <v>43910.298773148148</v>
+          </cell>
+          <cell r="M50" t="str">
             <v>PROOSGMM_CNM_COMPROBANTE</v>
           </cell>
-          <cell r="Q50" t="str">
-            <v>Ended OK</v>
+          <cell r="P50" t="str">
+            <v>Ended Not OK</v>
           </cell>
         </row>
         <row r="51">
           <cell r="A51" t="str">
-            <v>10885</v>
+            <v>30505</v>
           </cell>
           <cell r="E51">
-            <v>43869.290555555555</v>
+            <v>43910.288587962961</v>
           </cell>
           <cell r="I51">
-            <v>43869.303171296298</v>
-          </cell>
-          <cell r="N51" t="str">
-            <v>PROOSGMM_CNM_PADECIMIENTO</v>
-          </cell>
-          <cell r="Q51" t="str">
+            <v>43910.316724537035</v>
+          </cell>
+          <cell r="M51" t="str">
+            <v>PROOSGMM_CNM_SOLICITUD</v>
+          </cell>
+          <cell r="P51" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="52">
           <cell r="A52" t="str">
-            <v>10889</v>
+            <v>30506</v>
           </cell>
           <cell r="E52">
-            <v>43869.290555555555</v>
+            <v>43910.288587962961</v>
           </cell>
           <cell r="I52">
-            <v>43869.306018518517</v>
-          </cell>
-          <cell r="N52" t="str">
+            <v>43910.30673611111</v>
+          </cell>
+          <cell r="M52" t="str">
             <v>PROOSGMM_CNM_NOTAS_MEDICAS</v>
           </cell>
-          <cell r="Q52" t="str">
+          <cell r="P52" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="53">
           <cell r="A53" t="str">
-            <v>10884</v>
+            <v>30503</v>
           </cell>
           <cell r="E53">
-            <v>43869.290555555555</v>
+            <v>43910.288587962961</v>
           </cell>
           <cell r="I53">
-            <v>43869.317476851851</v>
-          </cell>
-          <cell r="N53" t="str">
-            <v>PROOSGMM_CNM_SOLICITUD</v>
-          </cell>
-          <cell r="Q53" t="str">
+            <v>43910.30259259259</v>
+          </cell>
+          <cell r="M53" t="str">
+            <v>PROOSGMM_CNM_PADECIMIENTO</v>
+          </cell>
+          <cell r="P53" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="54">
           <cell r="A54" t="str">
-            <v>19643</v>
+            <v>14256</v>
           </cell>
           <cell r="E54">
-            <v>43869.317488425928</v>
+            <v>43910.379837962966</v>
           </cell>
           <cell r="I54">
-            <v>43869.323125000003</v>
-          </cell>
-          <cell r="N54" t="str">
+            <v>43910.379861111112</v>
+          </cell>
+          <cell r="M54" t="str">
             <v>PROOSGMM_FYF_wkf_gmm_fyf_gd</v>
           </cell>
-          <cell r="Q54" t="str">
-            <v>Ended OK</v>
+          <cell r="P54" t="str">
+            <v>Ended Not OK</v>
           </cell>
         </row>
         <row r="55">
           <cell r="A55" t="str">
-            <v>1680</v>
+            <v>24013</v>
           </cell>
           <cell r="E55">
-            <v>43869.323136574072</v>
+            <v>43910.39199074074</v>
           </cell>
           <cell r="I55">
-            <v>43869.325474537036</v>
-          </cell>
-          <cell r="N55" t="str">
+            <v>43910.39340277778</v>
+          </cell>
+          <cell r="M55" t="str">
             <v>PROOSGMM_FYF_bq_fugasfraudesgmma</v>
           </cell>
-          <cell r="Q55" t="str">
+          <cell r="P55" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
         <row r="56">
           <cell r="A56" t="str">
-            <v>7589</v>
+            <v>28833</v>
           </cell>
           <cell r="E56">
-            <v>43869.325474537036</v>
+            <v>43910.393414351849</v>
           </cell>
           <cell r="I56">
-            <v>43869.335532407407</v>
-          </cell>
-          <cell r="N56" t="str">
+            <v>43910.40357638889</v>
+          </cell>
+          <cell r="M56" t="str">
             <v>PROOSGMM_FYF_sh_bq_fugasyfraudes</v>
           </cell>
-          <cell r="Q56" t="str">
+          <cell r="P56" t="str">
             <v>Ended OK</v>
           </cell>
         </row>
@@ -1507,7 +1507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DBE8FFA-39E3-4C76-A19E-70A580C87EF3}">
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F52"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1540,1173 +1542,1173 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>[1]Sheet1!A6</f>
-        <v>33548</v>
+        <v>18220</v>
       </c>
       <c r="B2" s="3">
         <f>[1]Sheet1!E6</f>
-        <v>43869.003472222219</v>
+        <v>43910.003472222219</v>
       </c>
       <c r="C2" s="3">
         <f>[1]Sheet1!I6</f>
-        <v>43869.048090277778</v>
+        <v>43910.059444444443</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="str">
-        <f>[1]Sheet1!N6</f>
-        <v>PROOSGMM_oinfo_FYF_01</v>
+        <f>[1]Sheet1!M6</f>
+        <v>PROOSGMM_oinfo_FYF_05</v>
       </c>
       <c r="F2" t="str">
-        <f>[1]Sheet1!Q6</f>
-        <v>Ended OK</v>
+        <f>[1]Sheet1!P6</f>
+        <v>Ended Not OK</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>[1]Sheet1!A7</f>
-        <v>33544</v>
+        <v>18208</v>
       </c>
       <c r="B3" s="3">
         <f>[1]Sheet1!E7</f>
-        <v>43869.003472222219</v>
+        <v>43910.003472222219</v>
       </c>
       <c r="C3" s="3">
         <f>[1]Sheet1!I7</f>
-        <v>43869.080069444448</v>
+        <v>43910.04378472222</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="str">
-        <f>[1]Sheet1!N7</f>
-        <v>PROOSGMM_oinfo_FYF_02</v>
+        <f>[1]Sheet1!M7</f>
+        <v>PROOSGMM_oinfo_FYF_03</v>
       </c>
       <c r="F3" t="str">
-        <f>[1]Sheet1!Q7</f>
-        <v>Ended OK</v>
+        <f>[1]Sheet1!P7</f>
+        <v>Ended Not OK</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>[1]Sheet1!A8</f>
-        <v>33549</v>
+        <v>18203</v>
       </c>
       <c r="B4" s="3">
         <f>[1]Sheet1!E8</f>
-        <v>43869.003472222219</v>
+        <v>43910.003472222219</v>
       </c>
       <c r="C4" s="3">
         <f>[1]Sheet1!I8</f>
-        <v>43869.094722222224</v>
+        <v>43910.041331018518</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="str">
-        <f>[1]Sheet1!N8</f>
-        <v>PROOSGMM_oinfo_FYF_05</v>
+        <f>[1]Sheet1!M8</f>
+        <v>PROOSGMM_oinfo_FYF_02</v>
       </c>
       <c r="F4" t="str">
-        <f>[1]Sheet1!Q8</f>
-        <v>Ended OK</v>
+        <f>[1]Sheet1!P8</f>
+        <v>Ended Not OK</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>[1]Sheet1!A9</f>
-        <v>33546</v>
+        <v>18202</v>
       </c>
       <c r="B5" s="3">
         <f>[1]Sheet1!E9</f>
-        <v>43869.003472222219</v>
+        <v>43910.003472222219</v>
       </c>
       <c r="C5" s="3">
         <f>[1]Sheet1!I9</f>
-        <v>43869.09746527778</v>
+        <v>43910.037870370368</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="str">
-        <f>[1]Sheet1!N9</f>
+        <f>[1]Sheet1!M9</f>
         <v>PROOSGMM_oinfo_FYF_04</v>
       </c>
       <c r="F5" t="str">
-        <f>[1]Sheet1!Q9</f>
-        <v>Ended OK</v>
+        <f>[1]Sheet1!P9</f>
+        <v>Ended Not OK</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>[1]Sheet1!A10</f>
-        <v>33547</v>
+        <v>18204</v>
       </c>
       <c r="B6" s="3">
         <f>[1]Sheet1!E10</f>
-        <v>43869.003472222219</v>
+        <v>43910.003472222219</v>
       </c>
       <c r="C6" s="3">
         <f>[1]Sheet1!I10</f>
-        <v>43869.104537037034</v>
+        <v>43910.027314814812</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="str">
-        <f>[1]Sheet1!N10</f>
-        <v>PROOSGMM_oinfo_FYF_03</v>
+        <f>[1]Sheet1!M10</f>
+        <v>PROOSGMM_oinfo_FYF_01</v>
       </c>
       <c r="F6" t="str">
-        <f>[1]Sheet1!Q10</f>
-        <v>Ended Not OK</v>
+        <f>[1]Sheet1!P10</f>
+        <v>Ended OK</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>[1]Sheet1!A11</f>
-        <v>37259</v>
+        <v>23380</v>
       </c>
       <c r="B7" s="3">
         <f>[1]Sheet1!E11</f>
-        <v>43869.006944444445</v>
+        <v>43910.006944444445</v>
       </c>
       <c r="C7" s="3">
         <f>[1]Sheet1!I11</f>
-        <v>43869.106203703705</v>
+        <v>43910.060833333337</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="str">
-        <f>[1]Sheet1!N11</f>
+        <f>[1]Sheet1!M11</f>
         <v>PROOSGMM_oinfo_GMM_05</v>
       </c>
       <c r="F7" t="str">
-        <f>[1]Sheet1!Q11</f>
-        <v>Ended OK</v>
+        <f>[1]Sheet1!P11</f>
+        <v>Ended Not OK</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>[1]Sheet1!A12</f>
-        <v>11230</v>
+        <v>10164</v>
       </c>
       <c r="B8" s="3">
         <f>[1]Sheet1!E12</f>
-        <v>43869.072916666664</v>
+        <v>43910.072916666664</v>
       </c>
       <c r="C8" s="3">
         <f>[1]Sheet1!I12</f>
-        <v>43869.139166666668</v>
+        <v>43910.12709490741</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="str">
-        <f>[1]Sheet1!N12</f>
+        <f>[1]Sheet1!M12</f>
         <v>PROOSGMM_oinfo_GMM_01</v>
       </c>
       <c r="F8" t="str">
-        <f>[1]Sheet1!Q12</f>
+        <f>[1]Sheet1!P12</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>[1]Sheet1!A13</f>
-        <v>23694</v>
+        <v>13695</v>
       </c>
       <c r="B9" s="3">
         <f>[1]Sheet1!E13</f>
-        <v>43869.083333333336</v>
+        <v>43910.083333333336</v>
       </c>
       <c r="C9" s="3">
         <f>[1]Sheet1!I13</f>
-        <v>43869.121215277781</v>
+        <v>43910.126747685186</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="str">
-        <f>[1]Sheet1!N13</f>
+        <f>[1]Sheet1!M13</f>
         <v>PROOSGMM_oinfo_GMM_04</v>
       </c>
       <c r="F9" t="str">
-        <f>[1]Sheet1!Q13</f>
+        <f>[1]Sheet1!P13</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>[1]Sheet1!A14</f>
-        <v>41191</v>
+        <v>21712</v>
       </c>
       <c r="B10" s="3">
         <f>[1]Sheet1!E14</f>
-        <v>43869.094722222224</v>
+        <v>43910.097222222219</v>
       </c>
       <c r="C10" s="3">
         <f>[1]Sheet1!I14</f>
-        <v>43869.120358796295</v>
+        <v>43910.176840277774</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="str">
-        <f>[1]Sheet1!N14</f>
-        <v>PROOSGMM_CNM_PROVEEDOR_MEDICO</v>
+        <f>[1]Sheet1!M14</f>
+        <v>PROOSEOT_extevo_EOT_301</v>
       </c>
       <c r="F10" t="str">
-        <f>[1]Sheet1!Q14</f>
+        <f>[1]Sheet1!P14</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>[1]Sheet1!A15</f>
-        <v>22688</v>
+        <v>21713</v>
       </c>
       <c r="B11" s="3">
         <f>[1]Sheet1!E15</f>
-        <v>43869.097222222219</v>
+        <v>43910.097222222219</v>
       </c>
       <c r="C11" s="3">
         <f>[1]Sheet1!I15</f>
-        <v>43869.140543981484</v>
+        <v>43910.134965277779</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" t="str">
-        <f>[1]Sheet1!N15</f>
+        <f>[1]Sheet1!M15</f>
         <v>PROOSEOT_extevo_EOT_101</v>
       </c>
       <c r="F11" t="str">
-        <f>[1]Sheet1!Q15</f>
+        <f>[1]Sheet1!P15</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>[1]Sheet1!A16</f>
-        <v>22689</v>
+        <v>32367</v>
       </c>
       <c r="B12" s="3">
         <f>[1]Sheet1!E16</f>
-        <v>43869.097222222219</v>
+        <v>43910.111111111109</v>
       </c>
       <c r="C12" s="3">
         <f>[1]Sheet1!I16</f>
-        <v>43869.183831018519</v>
+        <v>43910.116712962961</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" t="str">
-        <f>[1]Sheet1!N16</f>
-        <v>PROOSEOT_extevo_EOT_301</v>
+        <f>[1]Sheet1!M16</f>
+        <v>PROOSGMM_oinfo_GMM_06</v>
       </c>
       <c r="F12" t="str">
-        <f>[1]Sheet1!Q16</f>
+        <f>[1]Sheet1!P16</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
         <f>[1]Sheet1!A17</f>
-        <v>23706</v>
+        <v>10573</v>
       </c>
       <c r="B13" s="3">
         <f>[1]Sheet1!E17</f>
-        <v>43869.09747685185</v>
+        <v>43910.119444444441</v>
       </c>
       <c r="C13" s="3">
         <f>[1]Sheet1!I17</f>
-        <v>43869.13380787037</v>
+        <v>43910.12228009259</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" t="str">
-        <f>[1]Sheet1!N17</f>
-        <v>PROOSGMM_wkf_gmm_taller_producto</v>
+        <f>[1]Sheet1!M17</f>
+        <v>PROOSCRM_wkf_cat_padecimiento_icd9</v>
       </c>
       <c r="F13" t="str">
-        <f>[1]Sheet1!Q17</f>
+        <f>[1]Sheet1!P17</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
         <f>[1]Sheet1!A18</f>
-        <v>55825</v>
+        <v>11362</v>
       </c>
       <c r="B14" s="3">
         <f>[1]Sheet1!E18</f>
-        <v>43869.111111111109</v>
+        <v>43910.120138888888</v>
       </c>
       <c r="C14" s="3">
         <f>[1]Sheet1!I18</f>
-        <v>43869.117986111109</v>
+        <v>43910.122974537036</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" t="str">
-        <f>[1]Sheet1!N18</f>
-        <v>PROOSGMM_oinfo_GMM_06</v>
+        <f>[1]Sheet1!M18</f>
+        <v>PROOSCRM_wkf_cat_region_corporal</v>
       </c>
       <c r="F14" t="str">
-        <f>[1]Sheet1!Q18</f>
+        <f>[1]Sheet1!P18</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>[1]Sheet1!A19</f>
-        <v>683</v>
+        <v>16705</v>
       </c>
       <c r="B15" s="3">
         <f>[1]Sheet1!E19</f>
-        <v>43869.119444444441</v>
+        <v>43910.125694444447</v>
       </c>
       <c r="C15" s="3">
         <f>[1]Sheet1!I19</f>
-        <v>43869.12228009259</v>
+        <v>43910.128518518519</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" t="str">
-        <f>[1]Sheet1!N19</f>
-        <v>PROOSCRM_wkf_cat_padecimiento_icd9</v>
+        <f>[1]Sheet1!M19</f>
+        <v>PROOSCRM_wkf_cat_sistema_origen</v>
       </c>
       <c r="F15" t="str">
-        <f>[1]Sheet1!Q19</f>
+        <f>[1]Sheet1!P19</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>[1]Sheet1!A20</f>
-        <v>7177</v>
+        <v>17357</v>
       </c>
       <c r="B16" s="3">
         <f>[1]Sheet1!E20</f>
-        <v>43869.120138888888</v>
+        <v>43910.126388888886</v>
       </c>
       <c r="C16" s="3">
         <f>[1]Sheet1!I20</f>
-        <v>43869.122974537036</v>
+        <v>43910.129212962966</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" t="str">
-        <f>[1]Sheet1!N20</f>
-        <v>PROOSCRM_wkf_cat_region_corporal</v>
+        <f>[1]Sheet1!M20</f>
+        <v>PROOSCRM_wkf_cat_grupo_icd</v>
       </c>
       <c r="F16" t="str">
-        <f>[1]Sheet1!Q20</f>
+        <f>[1]Sheet1!P20</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>[1]Sheet1!A21</f>
-        <v>13711</v>
+        <v>24877</v>
       </c>
       <c r="B17" s="3">
         <f>[1]Sheet1!E21</f>
-        <v>43869.125694444447</v>
+        <v>43910.133634259262</v>
       </c>
       <c r="C17" s="3">
         <f>[1]Sheet1!I21</f>
-        <v>43869.128530092596</v>
+        <v>43910.162974537037</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" t="str">
-        <f>[1]Sheet1!N21</f>
-        <v>PROOSCRM_wkf_cat_sistema_origen</v>
+        <f>[1]Sheet1!M21</f>
+        <v>PROOSGMM_wkf_gmm_taller_producto</v>
       </c>
       <c r="F17" t="str">
-        <f>[1]Sheet1!Q21</f>
+        <f>[1]Sheet1!P21</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>[1]Sheet1!A22</f>
-        <v>14791</v>
+        <v>26051</v>
       </c>
       <c r="B18" s="3">
         <f>[1]Sheet1!E22</f>
-        <v>43869.126388888886</v>
+        <v>43910.134976851848</v>
       </c>
       <c r="C18" s="3">
         <f>[1]Sheet1!I22</f>
-        <v>43869.129224537035</v>
+        <v>43910.21738425926</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" t="str">
-        <f>[1]Sheet1!N22</f>
-        <v>PROOSCRM_wkf_cat_grupo_icd</v>
+        <f>[1]Sheet1!M22</f>
+        <v>PROOSEOT_extevo_EOT_251</v>
       </c>
       <c r="F18" t="str">
-        <f>[1]Sheet1!Q22</f>
+        <f>[1]Sheet1!P22</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>[1]Sheet1!A23</f>
-        <v>22741</v>
+        <v>7795</v>
       </c>
       <c r="B19" s="3">
         <f>[1]Sheet1!E23</f>
-        <v>43869.13380787037</v>
+        <v>43910.145833333336</v>
       </c>
       <c r="C19" s="3">
         <f>[1]Sheet1!I23</f>
-        <v>43869.147835648146</v>
+        <v>43910.218969907408</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" t="str">
-        <f>[1]Sheet1!N23</f>
-        <v>PROOSGMM_CNM_POLIZA</v>
+        <f>[1]Sheet1!M23</f>
+        <v>PROOSGMM_oinfo_GMM_02</v>
       </c>
       <c r="F19" t="str">
-        <f>[1]Sheet1!Q23</f>
+        <f>[1]Sheet1!P23</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>[1]Sheet1!A24</f>
-        <v>30508</v>
+        <v>25440</v>
       </c>
       <c r="B20" s="3">
         <f>[1]Sheet1!E24</f>
-        <v>43869.140555555554</v>
+        <v>43910.161111111112</v>
       </c>
       <c r="C20" s="3">
         <f>[1]Sheet1!I24</f>
-        <v>43869.227152777778</v>
+        <v>43910.182222222225</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" t="str">
-        <f>[1]Sheet1!N24</f>
-        <v>PROOSEOT_extevo_EOT_251</v>
+        <f>[1]Sheet1!M24</f>
+        <v>PROOSGMM_CNM_PROVEEDOR_MEDICO</v>
       </c>
       <c r="F20" t="str">
-        <f>[1]Sheet1!Q24</f>
+        <f>[1]Sheet1!P24</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>[1]Sheet1!A25</f>
-        <v>13972</v>
+        <v>22383</v>
       </c>
       <c r="B21" s="3">
         <f>[1]Sheet1!E25</f>
-        <v>43869.145833333336</v>
+        <v>43910.162986111114</v>
       </c>
       <c r="C21" s="3">
         <f>[1]Sheet1!I25</f>
-        <v>43869.218854166669</v>
+        <v>43910.179745370369</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" t="str">
-        <f>[1]Sheet1!N25</f>
-        <v>PROOSGMM_oinfo_GMM_02</v>
+        <f>[1]Sheet1!M25</f>
+        <v>PROOSGMM_CNM_POLIZA</v>
       </c>
       <c r="F21" t="str">
-        <f>[1]Sheet1!Q25</f>
+        <f>[1]Sheet1!P25</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>[1]Sheet1!A26</f>
-        <v>10111</v>
+        <v>25538</v>
       </c>
       <c r="B22" s="3">
         <f>[1]Sheet1!E26</f>
-        <v>43869.147835648146</v>
+        <v>43910.166666666664</v>
       </c>
       <c r="C22" s="3">
         <f>[1]Sheet1!I26</f>
-        <v>43869.193715277775</v>
+        <v>43910.173692129632</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" t="str">
-        <f>[1]Sheet1!N26</f>
-        <v>PROOSGMM_CNM_ASEG_DATOS_ADICIONALES</v>
+        <f>[1]Sheet1!M26</f>
+        <v>PROOSGMM_AZUL_wkf_gccticdc</v>
       </c>
       <c r="F22" t="str">
-        <f>[1]Sheet1!Q26</f>
+        <f>[1]Sheet1!P26</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
         <f>[1]Sheet1!A27</f>
-        <v>28289</v>
+        <v>25579</v>
       </c>
       <c r="B23" s="3">
         <f>[1]Sheet1!E27</f>
-        <v>43869.166666666664</v>
+        <v>43910.166666666664</v>
       </c>
       <c r="C23" s="3">
         <f>[1]Sheet1!I27</f>
-        <v>43869.172291666669</v>
+        <v>43910.173692129632</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" t="str">
-        <f>[1]Sheet1!N27</f>
-        <v>PROOSGMM_AZUL_wkf_gfvtcna0</v>
+        <f>[1]Sheet1!M27</f>
+        <v>PROOSGMM_AZUL_wkf_gfvtfla0</v>
       </c>
       <c r="F23" t="str">
-        <f>[1]Sheet1!Q27</f>
+        <f>[1]Sheet1!P27</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>[1]Sheet1!A28</f>
-        <v>28288</v>
+        <v>25535</v>
       </c>
       <c r="B24" s="3">
         <f>[1]Sheet1!E28</f>
-        <v>43869.166666666664</v>
+        <v>43910.166666666664</v>
       </c>
       <c r="C24" s="3">
         <f>[1]Sheet1!I28</f>
-        <v>43869.172291666669</v>
+        <v>43910.173692129632</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="str">
-        <f>[1]Sheet1!N28</f>
-        <v>PROOSGMM_AZUL_wkf_gfvtfla0</v>
+        <f>[1]Sheet1!M28</f>
+        <v>PROOSGMM_AZUL_wkf_gfvtcna0</v>
       </c>
       <c r="F24" t="str">
-        <f>[1]Sheet1!Q28</f>
+        <f>[1]Sheet1!P28</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>[1]Sheet1!A29</f>
-        <v>28290</v>
+        <v>25537</v>
       </c>
       <c r="B25" s="3">
         <f>[1]Sheet1!E29</f>
-        <v>43869.166666666664</v>
+        <v>43910.166666666664</v>
       </c>
       <c r="C25" s="3">
         <f>[1]Sheet1!I29</f>
-        <v>43869.172291666669</v>
+        <v>43910.173692129632</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" t="str">
-        <f>[1]Sheet1!N29</f>
-        <v>PROOSGMM_AZUL_wkf_gccticdc</v>
+        <f>[1]Sheet1!M29</f>
+        <v>PROOSGMM_AZUL_wkf_gfvtagt0</v>
       </c>
       <c r="F25" t="str">
-        <f>[1]Sheet1!Q29</f>
+        <f>[1]Sheet1!P29</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>[1]Sheet1!A30</f>
-        <v>28283</v>
+        <v>10837</v>
       </c>
       <c r="B26" s="3">
         <f>[1]Sheet1!E30</f>
-        <v>43869.166666666664</v>
+        <v>43910.176851851851</v>
       </c>
       <c r="C26" s="3">
         <f>[1]Sheet1!I30</f>
-        <v>43869.173692129632</v>
+        <v>43910.266215277778</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" t="str">
-        <f>[1]Sheet1!N30</f>
-        <v>PROOSGMM_AZUL_wkf_gfvtagt0</v>
+        <f>[1]Sheet1!M30</f>
+        <v>PROOSEOT_extevo_EOT_351</v>
       </c>
       <c r="F26" t="str">
-        <f>[1]Sheet1!Q30</f>
+        <f>[1]Sheet1!P30</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>[1]Sheet1!A31</f>
-        <v>16982</v>
+        <v>17690</v>
       </c>
       <c r="B27" s="3">
         <f>[1]Sheet1!E31</f>
-        <v>43869.183842592596</v>
+        <v>43910.179756944446</v>
       </c>
       <c r="C27" s="3">
         <f>[1]Sheet1!I31</f>
-        <v>43869.270416666666</v>
+        <v>43910.225752314815</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" t="str">
-        <f>[1]Sheet1!N31</f>
-        <v>PROOSEOT_extevo_EOT_351</v>
+        <f>[1]Sheet1!M31</f>
+        <v>PROOSGMM_CNM_ASEG_DATOS_ADICIONALES</v>
       </c>
       <c r="F27" t="str">
-        <f>[1]Sheet1!Q31</f>
+        <f>[1]Sheet1!P31</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>[1]Sheet1!A32</f>
-        <v>41190</v>
+        <v>51878</v>
       </c>
       <c r="B28" s="3">
         <f>[1]Sheet1!E32</f>
-        <v>43869.1875</v>
+        <v>43910.1875</v>
       </c>
       <c r="C28" s="3">
         <f>[1]Sheet1!I32</f>
-        <v>43869.190081018518</v>
+        <v>43910.190925925926</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" t="str">
-        <f>[1]Sheet1!N32</f>
+        <f>[1]Sheet1!M32</f>
         <v>PROOSGMM_BDM_valida_recla</v>
       </c>
       <c r="F28" t="str">
-        <f>[1]Sheet1!Q32</f>
+        <f>[1]Sheet1!P32</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>[1]Sheet1!A33</f>
-        <v>44852</v>
+        <v>1213</v>
       </c>
       <c r="B29" s="3">
         <f>[1]Sheet1!E33</f>
-        <v>43869.190092592595</v>
+        <v>43910.190937500003</v>
       </c>
       <c r="C29" s="3">
         <f>[1]Sheet1!I33</f>
-        <v>43869.207175925927</v>
+        <v>43910.237337962964</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" t="str">
-        <f>[1]Sheet1!N33</f>
-        <v>PROOSGMM_recla_LMP_NRLTRCL0</v>
+        <f>[1]Sheet1!M33</f>
+        <v>PROOSGMM_recla_LMP_NRLTSLR0</v>
       </c>
       <c r="F29" t="str">
-        <f>[1]Sheet1!Q33</f>
+        <f>[1]Sheet1!P33</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>[1]Sheet1!A34</f>
-        <v>44858</v>
+        <v>1214</v>
       </c>
       <c r="B30" s="3">
         <f>[1]Sheet1!E34</f>
-        <v>43869.190092592595</v>
+        <v>43910.190937500003</v>
       </c>
       <c r="C30" s="3">
         <f>[1]Sheet1!I34</f>
-        <v>43869.211759259262</v>
+        <v>43910.231736111113</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" t="str">
-        <f>[1]Sheet1!N34</f>
-        <v>PROOSGMM_recla_LMP_NRLTDDC0</v>
+        <f>[1]Sheet1!M34</f>
+        <v>PROOSGMM_recla_LMP_NRLTASP0</v>
       </c>
       <c r="F30" t="str">
-        <f>[1]Sheet1!Q34</f>
+        <f>[1]Sheet1!P34</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>[1]Sheet1!A35</f>
-        <v>44867</v>
+        <v>1222</v>
       </c>
       <c r="B31" s="3">
         <f>[1]Sheet1!E35</f>
-        <v>43869.190092592595</v>
+        <v>43910.190937500003</v>
       </c>
       <c r="C31" s="3">
         <f>[1]Sheet1!I35</f>
-        <v>43869.21638888889</v>
+        <v>43910.219398148147</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" t="str">
-        <f>[1]Sheet1!N35</f>
+        <f>[1]Sheet1!M35</f>
         <v>PROOSGMM_recla_LMP_NRLTAAN0</v>
       </c>
       <c r="F31" t="str">
-        <f>[1]Sheet1!Q35</f>
+        <f>[1]Sheet1!P35</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>[1]Sheet1!A36</f>
-        <v>44851</v>
+        <v>1218</v>
       </c>
       <c r="B32" s="3">
         <f>[1]Sheet1!E36</f>
-        <v>43869.190092592595</v>
+        <v>43910.190937500003</v>
       </c>
       <c r="C32" s="3">
         <f>[1]Sheet1!I36</f>
-        <v>43869.232615740744</v>
+        <v>43910.212361111109</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" t="str">
-        <f>[1]Sheet1!N36</f>
-        <v>PROOSGMM_recla_LMP_NRLTASP0</v>
+        <f>[1]Sheet1!M36</f>
+        <v>PROOSGMM_recla_LMP_NRLTRCL0</v>
       </c>
       <c r="F32" t="str">
-        <f>[1]Sheet1!Q36</f>
+        <f>[1]Sheet1!P36</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>[1]Sheet1!A37</f>
-        <v>44856</v>
+        <v>1212</v>
       </c>
       <c r="B33" s="3">
         <f>[1]Sheet1!E37</f>
-        <v>43869.190092592595</v>
+        <v>43910.190937500003</v>
       </c>
       <c r="C33" s="3">
         <f>[1]Sheet1!I37</f>
-        <v>43869.232743055552</v>
+        <v>43910.212384259263</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" t="str">
-        <f>[1]Sheet1!N37</f>
-        <v>PROOSGMM_recla_LMP_NRLTSLR0</v>
+        <f>[1]Sheet1!M37</f>
+        <v>PROOSGMM_recla_LMP_NRLTCMP0</v>
       </c>
       <c r="F33" t="str">
-        <f>[1]Sheet1!Q37</f>
+        <f>[1]Sheet1!P37</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
         <f>[1]Sheet1!A38</f>
-        <v>44855</v>
+        <v>1217</v>
       </c>
       <c r="B34" s="3">
         <f>[1]Sheet1!E38</f>
-        <v>43869.190092592595</v>
+        <v>43910.190937500003</v>
       </c>
       <c r="C34" s="3">
         <f>[1]Sheet1!I38</f>
-        <v>43869.245648148149</v>
+        <v>43910.195717592593</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" t="str">
-        <f>[1]Sheet1!N38</f>
-        <v>PROOSGMM_recla_LMP_NRLTCMP0</v>
+        <f>[1]Sheet1!M38</f>
+        <v>PROOSGMM_recla_LMP_NRLTDDC0</v>
       </c>
       <c r="F34" t="str">
-        <f>[1]Sheet1!Q38</f>
-        <v>Ended OK</v>
+        <f>[1]Sheet1!P38</f>
+        <v>Ended Not OK</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>[1]Sheet1!A39</f>
-        <v>1435</v>
+        <v>18899</v>
       </c>
       <c r="B35" s="3">
         <f>[1]Sheet1!E39</f>
-        <v>43869.193726851852</v>
+        <v>43910.225763888891</v>
       </c>
       <c r="C35" s="3">
         <f>[1]Sheet1!I39</f>
-        <v>43869.23165509259</v>
+        <v>43910.272037037037</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" t="str">
-        <f>[1]Sheet1!N39</f>
+        <f>[1]Sheet1!M39</f>
         <v>PROOSGMM_CNM_COBERT_DATOS_ADICIONALES</v>
       </c>
       <c r="F35" t="str">
-        <f>[1]Sheet1!Q39</f>
+        <f>[1]Sheet1!P39</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>[1]Sheet1!A40</f>
-        <v>2070</v>
+        <v>28882</v>
       </c>
       <c r="B36" s="3">
         <f>[1]Sheet1!E40</f>
-        <v>43869.231666666667</v>
+        <v>43910.231747685182</v>
       </c>
       <c r="C36" s="3">
         <f>[1]Sheet1!I40</f>
-        <v>43869.248240740744</v>
+        <v>43910.248495370368</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" t="str">
-        <f>[1]Sheet1!N40</f>
-        <v>PROOSGMM_CNM_POLIZA_DATOS_ADICIONALES</v>
+        <f>[1]Sheet1!M40</f>
+        <v>PROOSGMM_CNM_RECLAMACION</v>
       </c>
       <c r="F36" t="str">
-        <f>[1]Sheet1!Q40</f>
+        <f>[1]Sheet1!P40</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>[1]Sheet1!A41</f>
-        <v>2653</v>
+        <v>31926</v>
       </c>
       <c r="B37" s="3">
         <f>[1]Sheet1!E41</f>
-        <v>43869.232615740744</v>
+        <v>43910.232638888891</v>
       </c>
       <c r="C37" s="3">
         <f>[1]Sheet1!I41</f>
-        <v>43869.242407407408</v>
+        <v>43910.275277777779</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" t="str">
-        <f>[1]Sheet1!N41</f>
-        <v>PROOSGMM_CNM_RECLAMACION</v>
+        <f>[1]Sheet1!M41</f>
+        <v>PROOSGMM_orecla_LMP</v>
       </c>
       <c r="F37" t="str">
-        <f>[1]Sheet1!Q41</f>
+        <f>[1]Sheet1!P41</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>[1]Sheet1!A42</f>
-        <v>24197</v>
+        <v>39835</v>
       </c>
       <c r="B38" s="3">
         <f>[1]Sheet1!E42</f>
-        <v>43869.245659722219</v>
+        <v>43910.237349537034</v>
       </c>
       <c r="C38" s="3">
         <f>[1]Sheet1!I42</f>
-        <v>43869.261770833335</v>
+        <v>43910.318437499998</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" t="str">
-        <f>[1]Sheet1!N42</f>
-        <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_GC</v>
+        <f>[1]Sheet1!M42</f>
+        <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_DG</v>
       </c>
       <c r="F38" t="str">
-        <f>[1]Sheet1!Q42</f>
+        <f>[1]Sheet1!P42</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>[1]Sheet1!A43</f>
-        <v>24187</v>
+        <v>39839</v>
       </c>
       <c r="B39" s="3">
         <f>[1]Sheet1!E43</f>
-        <v>43869.245659722219</v>
+        <v>43910.237349537034</v>
       </c>
       <c r="C39" s="3">
         <f>[1]Sheet1!I43</f>
-        <v>43869.272488425922</v>
+        <v>43910.288587962961</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" t="str">
-        <f>[1]Sheet1!N43</f>
-        <v>PROOSGMM_orecla_LMP</v>
+        <f>[1]Sheet1!M43</f>
+        <v>PROOSGMM_ENR_SOLICITUD</v>
       </c>
       <c r="F39" t="str">
-        <f>[1]Sheet1!Q43</f>
+        <f>[1]Sheet1!P43</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>[1]Sheet1!A44</f>
-        <v>24188</v>
+        <v>39838</v>
       </c>
       <c r="B40" s="3">
         <f>[1]Sheet1!E44</f>
-        <v>43869.245659722219</v>
+        <v>43910.237349537034</v>
       </c>
       <c r="C40" s="3">
         <f>[1]Sheet1!I44</f>
-        <v>43869.282430555555</v>
+        <v>43910.278726851851</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" t="str">
-        <f>[1]Sheet1!N44</f>
+        <f>[1]Sheet1!M44</f>
         <v>PROOSGMM_ENR_SOLICITUD_DG</v>
       </c>
       <c r="F40" t="str">
-        <f>[1]Sheet1!Q44</f>
+        <f>[1]Sheet1!P44</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
         <f>[1]Sheet1!A45</f>
-        <v>24186</v>
+        <v>39834</v>
       </c>
       <c r="B41" s="3">
         <f>[1]Sheet1!E45</f>
-        <v>43869.245659722219</v>
+        <v>43910.237349537034</v>
       </c>
       <c r="C41" s="3">
         <f>[1]Sheet1!I45</f>
-        <v>43869.290543981479</v>
+        <v>43910.256076388891</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" t="str">
-        <f>[1]Sheet1!N45</f>
-        <v>PROOSGMM_ENR_SOLICITUD</v>
+        <f>[1]Sheet1!M45</f>
+        <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_GC</v>
       </c>
       <c r="F41" t="str">
-        <f>[1]Sheet1!Q45</f>
+        <f>[1]Sheet1!P45</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
         <f>[1]Sheet1!A46</f>
-        <v>24192</v>
+        <v>1923</v>
       </c>
       <c r="B42" s="3">
         <f>[1]Sheet1!E46</f>
-        <v>43869.245659722219</v>
+        <v>43910.263888888891</v>
       </c>
       <c r="C42" s="3">
         <f>[1]Sheet1!I46</f>
-        <v>43869.320798611108</v>
+        <v>43910.329768518517</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" t="str">
-        <f>[1]Sheet1!N46</f>
-        <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_DG</v>
+        <f>[1]Sheet1!M46</f>
+        <v>PROOSGMM_oinfo_GMM_03</v>
       </c>
       <c r="F42" t="str">
-        <f>[1]Sheet1!Q46</f>
+        <f>[1]Sheet1!P46</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
         <f>[1]Sheet1!A47</f>
-        <v>45415</v>
+        <v>29026</v>
       </c>
       <c r="B43" s="3">
         <f>[1]Sheet1!E47</f>
-        <v>43869.263888888891</v>
+        <v>43910.272037037037</v>
       </c>
       <c r="C43" s="3">
         <f>[1]Sheet1!I47</f>
-        <v>43869.322800925926</v>
+        <v>43910.294178240743</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" t="str">
-        <f>[1]Sheet1!N47</f>
-        <v>PROOSGMM_oinfo_GMM_03</v>
+        <f>[1]Sheet1!M47</f>
+        <v>PROOSGMM_CNM_POLIZA_DATOS_ADICIONALES</v>
       </c>
       <c r="F43" t="str">
-        <f>[1]Sheet1!Q47</f>
+        <f>[1]Sheet1!P47</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
         <f>[1]Sheet1!A48</f>
-        <v>9507</v>
+        <v>31171</v>
       </c>
       <c r="B44" s="3">
         <f>[1]Sheet1!E48</f>
-        <v>43869.272499999999</v>
+        <v>43910.275277777779</v>
       </c>
       <c r="C44" s="3">
         <f>[1]Sheet1!I48</f>
-        <v>43869.296967592592</v>
+        <v>43910.297407407408</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" t="str">
-        <f>[1]Sheet1!N48</f>
+        <f>[1]Sheet1!M48</f>
         <v>PROOSGMM_CNM_RECLAMACION_ACUMULADO</v>
       </c>
       <c r="F44" t="str">
-        <f>[1]Sheet1!Q48</f>
+        <f>[1]Sheet1!P48</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>[1]Sheet1!A49</f>
-        <v>53006</v>
+        <v>8254</v>
       </c>
       <c r="B45" s="3">
         <f>[1]Sheet1!E49</f>
-        <v>43869.28125</v>
+        <v>43910.28125</v>
       </c>
       <c r="C45" s="3">
         <f>[1]Sheet1!I49</f>
-        <v>43869.288506944446</v>
+        <v>43910.287557870368</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" t="str">
-        <f>[1]Sheet1!N49</f>
+        <f>[1]Sheet1!M49</f>
         <v>PROOSGMM_orecla_01</v>
       </c>
       <c r="F45" t="str">
-        <f>[1]Sheet1!Q49</f>
+        <f>[1]Sheet1!P49</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>[1]Sheet1!A50</f>
-        <v>32105</v>
+        <v>25039</v>
       </c>
       <c r="B46" s="3">
         <f>[1]Sheet1!E50</f>
-        <v>43869.288506944446</v>
+        <v>43910.287557870368</v>
       </c>
       <c r="C46" s="3">
         <f>[1]Sheet1!I50</f>
-        <v>43869.3125</v>
+        <v>43910.298773148148</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" t="str">
-        <f>[1]Sheet1!N50</f>
+        <f>[1]Sheet1!M50</f>
         <v>PROOSGMM_CNM_COMPROBANTE</v>
       </c>
       <c r="F46" t="str">
-        <f>[1]Sheet1!Q50</f>
-        <v>Ended OK</v>
+        <f>[1]Sheet1!P50</f>
+        <v>Ended Not OK</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>[1]Sheet1!A51</f>
-        <v>10885</v>
+        <v>30505</v>
       </c>
       <c r="B47" s="3">
         <f>[1]Sheet1!E51</f>
-        <v>43869.290555555555</v>
+        <v>43910.288587962961</v>
       </c>
       <c r="C47" s="3">
         <f>[1]Sheet1!I51</f>
-        <v>43869.303171296298</v>
+        <v>43910.316724537035</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" t="str">
-        <f>[1]Sheet1!N51</f>
-        <v>PROOSGMM_CNM_PADECIMIENTO</v>
+        <f>[1]Sheet1!M51</f>
+        <v>PROOSGMM_CNM_SOLICITUD</v>
       </c>
       <c r="F47" t="str">
-        <f>[1]Sheet1!Q51</f>
+        <f>[1]Sheet1!P51</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>[1]Sheet1!A52</f>
-        <v>10889</v>
+        <v>30506</v>
       </c>
       <c r="B48" s="3">
         <f>[1]Sheet1!E52</f>
-        <v>43869.290555555555</v>
+        <v>43910.288587962961</v>
       </c>
       <c r="C48" s="3">
         <f>[1]Sheet1!I52</f>
-        <v>43869.306018518517</v>
+        <v>43910.30673611111</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" t="str">
-        <f>[1]Sheet1!N52</f>
+        <f>[1]Sheet1!M52</f>
         <v>PROOSGMM_CNM_NOTAS_MEDICAS</v>
       </c>
       <c r="F48" t="str">
-        <f>[1]Sheet1!Q52</f>
+        <f>[1]Sheet1!P52</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>[1]Sheet1!A53</f>
-        <v>10884</v>
+        <v>30503</v>
       </c>
       <c r="B49" s="3">
         <f>[1]Sheet1!E53</f>
-        <v>43869.290555555555</v>
+        <v>43910.288587962961</v>
       </c>
       <c r="C49" s="3">
         <f>[1]Sheet1!I53</f>
-        <v>43869.317476851851</v>
+        <v>43910.30259259259</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" t="str">
-        <f>[1]Sheet1!N53</f>
-        <v>PROOSGMM_CNM_SOLICITUD</v>
+        <f>[1]Sheet1!M53</f>
+        <v>PROOSGMM_CNM_PADECIMIENTO</v>
       </c>
       <c r="F49" t="str">
-        <f>[1]Sheet1!Q53</f>
+        <f>[1]Sheet1!P53</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>[1]Sheet1!A54</f>
-        <v>19643</v>
+        <v>14256</v>
       </c>
       <c r="B50" s="3">
         <f>[1]Sheet1!E54</f>
-        <v>43869.317488425928</v>
+        <v>43910.379837962966</v>
       </c>
       <c r="C50" s="3">
         <f>[1]Sheet1!I54</f>
-        <v>43869.323125000003</v>
+        <v>43910.379861111112</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" t="str">
-        <f>[1]Sheet1!N54</f>
+        <f>[1]Sheet1!M54</f>
         <v>PROOSGMM_FYF_wkf_gmm_fyf_gd</v>
       </c>
       <c r="F50" t="str">
-        <f>[1]Sheet1!Q54</f>
-        <v>Ended OK</v>
+        <f>[1]Sheet1!P54</f>
+        <v>Ended Not OK</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>[1]Sheet1!A55</f>
-        <v>1680</v>
+        <v>24013</v>
       </c>
       <c r="B51" s="3">
         <f>[1]Sheet1!E55</f>
-        <v>43869.323136574072</v>
+        <v>43910.39199074074</v>
       </c>
       <c r="C51" s="3">
         <f>[1]Sheet1!I55</f>
-        <v>43869.325474537036</v>
+        <v>43910.39340277778</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" t="str">
-        <f>[1]Sheet1!N55</f>
+        <f>[1]Sheet1!M55</f>
         <v>PROOSGMM_FYF_bq_fugasfraudesgmma</v>
       </c>
       <c r="F51" t="str">
-        <f>[1]Sheet1!Q55</f>
+        <f>[1]Sheet1!P55</f>
         <v>Ended OK</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>[1]Sheet1!A56</f>
-        <v>7589</v>
+        <v>28833</v>
       </c>
       <c r="B52" s="3">
         <f>[1]Sheet1!E56</f>
-        <v>43869.325474537036</v>
+        <v>43910.393414351849</v>
       </c>
       <c r="C52" s="3">
         <f>[1]Sheet1!I56</f>
-        <v>43869.335532407407</v>
+        <v>43910.40357638889</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" t="str">
-        <f>[1]Sheet1!N56</f>
+        <f>[1]Sheet1!M56</f>
         <v>PROOSGMM_FYF_sh_bq_fugasyfraudes</v>
       </c>
       <c r="F52" t="str">
-        <f>[1]Sheet1!Q56</f>
+        <f>[1]Sheet1!P56</f>
         <v>Ended OK</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se agrega respaldo de maguero Audita tablas
</commit_message>
<xml_diff>
--- a/Malla/Malla.xlsx
+++ b/Malla/Malla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arturo\Documents\trendit\Malla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\trendit\Malla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4715F499-4F0F-43C2-B46F-ED2D4B3974E6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{850D2C12-5268-422C-996D-B7B12733F8FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CE728E4A-D156-4FB4-96FF-41168B829F56}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CE728E4A-D156-4FB4-96FF-41168B829F56}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,18 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -337,118 +345,118 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="A6" t="str">
-            <v>4700</v>
+            <v>40298</v>
           </cell>
           <cell r="E6">
-            <v>43913.003472222219</v>
+            <v>43917.003472222219</v>
           </cell>
           <cell r="I6">
-            <v>43913.006030092591</v>
+            <v>43917.039525462962</v>
           </cell>
           <cell r="M6" t="str">
-            <v>PROOSGMM_oinfo_FYF_02</v>
+            <v>PROOSGMM_oinfo_FYF_01</v>
           </cell>
           <cell r="P6" t="str">
-            <v>Ended Not OK</v>
+            <v>Ended OK</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7" t="str">
-            <v>4705</v>
+            <v>40299</v>
           </cell>
           <cell r="E7">
-            <v>43913.003472222219</v>
+            <v>43917.003472222219</v>
           </cell>
           <cell r="I7">
-            <v>43913.011481481481</v>
+            <v>43917.05537037037</v>
           </cell>
           <cell r="M7" t="str">
-            <v>PROOSGMM_oinfo_FYF_04</v>
+            <v>PROOSGMM_oinfo_FYF_02</v>
           </cell>
           <cell r="P7" t="str">
-            <v>Ended Not OK</v>
+            <v>Ended OK</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8" t="str">
-            <v>4699</v>
+            <v>40304</v>
           </cell>
           <cell r="E8">
-            <v>43913.003472222219</v>
+            <v>43917.003472222219</v>
           </cell>
           <cell r="I8">
-            <v>43913.018564814818</v>
+            <v>43917.05878472222</v>
           </cell>
           <cell r="M8" t="str">
-            <v>PROOSGMM_oinfo_FYF_01</v>
+            <v>PROOSGMM_oinfo_FYF_04</v>
           </cell>
           <cell r="P8" t="str">
-            <v>Ended Not OK</v>
+            <v>Ended OK</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9" t="str">
-            <v>4706</v>
+            <v>40300</v>
           </cell>
           <cell r="E9">
-            <v>43913.003472222219</v>
+            <v>43917.003472222219</v>
           </cell>
           <cell r="I9">
-            <v>43913.037002314813</v>
+            <v>43917.062048611115</v>
           </cell>
           <cell r="M9" t="str">
             <v>PROOSGMM_oinfo_FYF_03</v>
           </cell>
           <cell r="P9" t="str">
-            <v>Ended Not OK</v>
+            <v>Ended OK</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10" t="str">
-            <v>4701</v>
+            <v>40306</v>
           </cell>
           <cell r="E10">
-            <v>43913.003472222219</v>
+            <v>43917.003472222219</v>
           </cell>
           <cell r="I10">
-            <v>43913.061215277776</v>
+            <v>43917.075277777774</v>
           </cell>
           <cell r="M10" t="str">
             <v>PROOSGMM_oinfo_FYF_05</v>
           </cell>
           <cell r="P10" t="str">
-            <v>Ended Not OK</v>
+            <v>Ended OK</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11" t="str">
-            <v>10014</v>
+            <v>44089</v>
           </cell>
           <cell r="E11">
-            <v>43913.006944444445</v>
+            <v>43917.006944444445</v>
           </cell>
           <cell r="I11">
-            <v>43913.070925925924</v>
+            <v>43917.080370370371</v>
           </cell>
           <cell r="M11" t="str">
             <v>PROOSGMM_oinfo_GMM_05</v>
           </cell>
           <cell r="P11" t="str">
-            <v>Ended Not OK</v>
+            <v>Ended OK</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12" t="str">
-            <v>57093</v>
+            <v>28966</v>
           </cell>
           <cell r="E12">
-            <v>43913.072916666664</v>
+            <v>43917.058796296296</v>
           </cell>
           <cell r="I12">
-            <v>43913.136157407411</v>
+            <v>43917.085358796299</v>
           </cell>
           <cell r="M12" t="str">
-            <v>PROOSGMM_oinfo_GMM_01</v>
+            <v>PROOSGMM_wkf_gmm_taller_producto</v>
           </cell>
           <cell r="P12" t="str">
             <v>Ended OK</v>
@@ -456,16 +464,16 @@
         </row>
         <row r="13">
           <cell r="A13" t="str">
-            <v>9694</v>
+            <v>39255</v>
           </cell>
           <cell r="E13">
-            <v>43913.083333333336</v>
+            <v>43917.075289351851</v>
           </cell>
           <cell r="I13">
-            <v>43913.128287037034</v>
+            <v>43917.096817129626</v>
           </cell>
           <cell r="M13" t="str">
-            <v>PROOSGMM_oinfo_GMM_04</v>
+            <v>PROOSGMM_CNM_PROVEEDOR_MEDICO</v>
           </cell>
           <cell r="P13" t="str">
             <v>Ended OK</v>
@@ -473,16 +481,16 @@
         </row>
         <row r="14">
           <cell r="A14" t="str">
-            <v>24352</v>
+            <v>4468</v>
           </cell>
           <cell r="E14">
-            <v>43913.097222222219</v>
+            <v>43917.111111111109</v>
           </cell>
           <cell r="I14">
-            <v>43913.147534722222</v>
+            <v>43917.117361111108</v>
           </cell>
           <cell r="M14" t="str">
-            <v>PROOSEOT_extevo_EOT_101</v>
+            <v>PROOSGMM_oinfo_GMM_06</v>
           </cell>
           <cell r="P14" t="str">
             <v>Ended OK</v>
@@ -490,16 +498,16 @@
         </row>
         <row r="15">
           <cell r="A15" t="str">
-            <v>24353</v>
+            <v>28901</v>
           </cell>
           <cell r="E15">
-            <v>43913.097222222219</v>
+            <v>43917.119444444441</v>
           </cell>
           <cell r="I15">
-            <v>43913.186620370368</v>
+            <v>43917.12228009259</v>
           </cell>
           <cell r="M15" t="str">
-            <v>PROOSEOT_extevo_EOT_301</v>
+            <v>PROOSCRM_wkf_cat_padecimiento_icd9</v>
           </cell>
           <cell r="P15" t="str">
             <v>Ended OK</v>
@@ -507,16 +515,16 @@
         </row>
         <row r="16">
           <cell r="A16" t="str">
-            <v>37411</v>
+            <v>29999</v>
           </cell>
           <cell r="E16">
-            <v>43913.111111111109</v>
+            <v>43917.120138888888</v>
           </cell>
           <cell r="I16">
-            <v>43913.1171875</v>
+            <v>43917.122974537036</v>
           </cell>
           <cell r="M16" t="str">
-            <v>PROOSGMM_oinfo_GMM_06</v>
+            <v>PROOSCRM_wkf_cat_region_corporal</v>
           </cell>
           <cell r="P16" t="str">
             <v>Ended OK</v>
@@ -524,16 +532,16 @@
         </row>
         <row r="17">
           <cell r="A17" t="str">
-            <v>13190</v>
+            <v>37232</v>
           </cell>
           <cell r="E17">
-            <v>43913.119444444441</v>
+            <v>43917.072916666664</v>
           </cell>
           <cell r="I17">
-            <v>43913.12228009259</v>
+            <v>43917.124016203707</v>
           </cell>
           <cell r="M17" t="str">
-            <v>PROOSCRM_wkf_cat_padecimiento_icd9</v>
+            <v>PROOSGMM_oinfo_GMM_01</v>
           </cell>
           <cell r="P17" t="str">
             <v>Ended OK</v>
@@ -541,16 +549,16 @@
         </row>
         <row r="18">
           <cell r="A18" t="str">
-            <v>13957</v>
+            <v>44370</v>
           </cell>
           <cell r="E18">
-            <v>43913.120138888888</v>
+            <v>43917.083333333336</v>
           </cell>
           <cell r="I18">
-            <v>43913.122974537036</v>
+            <v>43917.124432870369</v>
           </cell>
           <cell r="M18" t="str">
-            <v>PROOSCRM_wkf_cat_region_corporal</v>
+            <v>PROOSGMM_oinfo_GMM_04</v>
           </cell>
           <cell r="P18" t="str">
             <v>Ended OK</v>
@@ -558,13 +566,13 @@
         </row>
         <row r="19">
           <cell r="A19" t="str">
-            <v>19759</v>
+            <v>3315</v>
           </cell>
           <cell r="E19">
-            <v>43913.125694444447</v>
+            <v>43917.125694444447</v>
           </cell>
           <cell r="I19">
-            <v>43913.128530092596</v>
+            <v>43917.128530092596</v>
           </cell>
           <cell r="M19" t="str">
             <v>PROOSCRM_wkf_cat_sistema_origen</v>
@@ -575,13 +583,13 @@
         </row>
         <row r="20">
           <cell r="A20" t="str">
-            <v>20795</v>
+            <v>4083</v>
           </cell>
           <cell r="E20">
-            <v>43913.126388888886</v>
+            <v>43917.126388888886</v>
           </cell>
           <cell r="I20">
-            <v>43913.129224537035</v>
+            <v>43917.129224537035</v>
           </cell>
           <cell r="M20" t="str">
             <v>PROOSCRM_wkf_cat_grupo_icd</v>
@@ -592,16 +600,16 @@
         </row>
         <row r="21">
           <cell r="A21" t="str">
-            <v>30422</v>
+            <v>26978</v>
           </cell>
           <cell r="E21">
-            <v>43913.136562500003</v>
+            <v>43917.116932870369</v>
           </cell>
           <cell r="I21">
-            <v>43913.178472222222</v>
+            <v>43917.132303240738</v>
           </cell>
           <cell r="M21" t="str">
-            <v>PROOSGMM_wkf_gmm_taller_producto</v>
+            <v>PROOSGMM_CNM_POLIZA</v>
           </cell>
           <cell r="P21" t="str">
             <v>Ended OK</v>
@@ -609,16 +617,16 @@
         </row>
         <row r="22">
           <cell r="A22" t="str">
-            <v>11590</v>
+            <v>12774</v>
           </cell>
           <cell r="E22">
-            <v>43913.137326388889</v>
+            <v>43917.097222222219</v>
           </cell>
           <cell r="I22">
-            <v>43913.161597222221</v>
+            <v>43917.134965277779</v>
           </cell>
           <cell r="M22" t="str">
-            <v>PROOSGMM_CNM_PROVEEDOR_MEDICO</v>
+            <v>PROOSEOT_extevo_EOT_101</v>
           </cell>
           <cell r="P22" t="str">
             <v>Ended OK</v>
@@ -626,16 +634,16 @@
         </row>
         <row r="23">
           <cell r="A23" t="str">
-            <v>18113</v>
+            <v>9849</v>
           </cell>
           <cell r="E23">
-            <v>43913.145833333336</v>
+            <v>43917.132303240738</v>
           </cell>
           <cell r="I23">
-            <v>43913.224699074075</v>
+            <v>43917.167164351849</v>
           </cell>
           <cell r="M23" t="str">
-            <v>PROOSGMM_oinfo_GMM_02</v>
+            <v>PROOSGMM_CNM_ASEG_DATOS_ADICIONALES</v>
           </cell>
           <cell r="P23" t="str">
             <v>Ended OK</v>
@@ -643,16 +651,16 @@
         </row>
         <row r="24">
           <cell r="A24" t="str">
-            <v>13099</v>
+            <v>12775</v>
           </cell>
           <cell r="E24">
-            <v>43913.147546296299</v>
+            <v>43917.097222222219</v>
           </cell>
           <cell r="I24">
-            <v>43913.229953703703</v>
+            <v>43917.171261574076</v>
           </cell>
           <cell r="M24" t="str">
-            <v>PROOSEOT_extevo_EOT_251</v>
+            <v>PROOSEOT_extevo_EOT_301</v>
           </cell>
           <cell r="P24" t="str">
             <v>Ended OK</v>
@@ -660,16 +668,16 @@
         </row>
         <row r="25">
           <cell r="A25" t="str">
-            <v>16328</v>
+            <v>19529</v>
           </cell>
           <cell r="E25">
-            <v>43913.166666666664</v>
+            <v>43917.166666666664</v>
           </cell>
           <cell r="I25">
-            <v>43913.172291666669</v>
+            <v>43917.175081018519</v>
           </cell>
           <cell r="M25" t="str">
-            <v>PROOSGMM_AZUL_wkf_gfvtagt0</v>
+            <v>PROOSGMM_AZUL_wkf_gccticdc</v>
           </cell>
           <cell r="P25" t="str">
             <v>Ended OK</v>
@@ -677,16 +685,16 @@
         </row>
         <row r="26">
           <cell r="A26" t="str">
-            <v>16331</v>
+            <v>19559</v>
           </cell>
           <cell r="E26">
-            <v>43913.166666666664</v>
+            <v>43917.166666666664</v>
           </cell>
           <cell r="I26">
-            <v>43913.172291666669</v>
+            <v>43917.176481481481</v>
           </cell>
           <cell r="M26" t="str">
-            <v>PROOSGMM_AZUL_wkf_gfvtcna0</v>
+            <v>PROOSGMM_AZUL_wkf_gfvtagt0</v>
           </cell>
           <cell r="P26" t="str">
             <v>Ended OK</v>
@@ -694,16 +702,16 @@
         </row>
         <row r="27">
           <cell r="A27" t="str">
-            <v>16330</v>
+            <v>19581</v>
           </cell>
           <cell r="E27">
-            <v>43913.166666666664</v>
+            <v>43917.166666666664</v>
           </cell>
           <cell r="I27">
-            <v>43913.172291666669</v>
+            <v>43917.176481481481</v>
           </cell>
           <cell r="M27" t="str">
-            <v>PROOSGMM_AZUL_wkf_gfvtfla0</v>
+            <v>PROOSGMM_AZUL_wkf_gfvtcna0</v>
           </cell>
           <cell r="P27" t="str">
             <v>Ended OK</v>
@@ -711,16 +719,16 @@
         </row>
         <row r="28">
           <cell r="A28" t="str">
-            <v>16329</v>
+            <v>19558</v>
           </cell>
           <cell r="E28">
-            <v>43913.166666666664</v>
+            <v>43917.166666666664</v>
           </cell>
           <cell r="I28">
-            <v>43913.172291666669</v>
+            <v>43917.179270833331</v>
           </cell>
           <cell r="M28" t="str">
-            <v>PROOSGMM_AZUL_wkf_gccticdc</v>
+            <v>PROOSGMM_AZUL_wkf_gfvtfla0</v>
           </cell>
           <cell r="P28" t="str">
             <v>Ended OK</v>
@@ -728,16 +736,16 @@
         </row>
         <row r="29">
           <cell r="A29" t="str">
-            <v>1431</v>
+            <v>53798</v>
           </cell>
           <cell r="E29">
-            <v>43913.178483796299</v>
+            <v>43917.191111111111</v>
           </cell>
           <cell r="I29">
-            <v>43913.191064814811</v>
+            <v>43917.193773148145</v>
           </cell>
           <cell r="M29" t="str">
-            <v>PROOSGMM_CNM_POLIZA</v>
+            <v>PROOSGMM_BDM_valida_recla</v>
           </cell>
           <cell r="P29" t="str">
             <v>Ended OK</v>
@@ -745,16 +753,16 @@
         </row>
         <row r="30">
           <cell r="A30" t="str">
-            <v>8781</v>
+            <v>56945</v>
           </cell>
           <cell r="E30">
-            <v>43913.186631944445</v>
+            <v>43917.193773148145</v>
           </cell>
           <cell r="I30">
-            <v>43913.273206018515</v>
+            <v>43917.20952546296</v>
           </cell>
           <cell r="M30" t="str">
-            <v>PROOSEOT_extevo_EOT_351</v>
+            <v>PROOSGMM_recla_LMP_NRLTRCL0</v>
           </cell>
           <cell r="P30" t="str">
             <v>Ended OK</v>
@@ -762,16 +770,16 @@
         </row>
         <row r="31">
           <cell r="A31" t="str">
-            <v>3203</v>
+            <v>56935</v>
           </cell>
           <cell r="E31">
-            <v>43913.1875</v>
+            <v>43917.193773148145</v>
           </cell>
           <cell r="I31">
-            <v>43913.18986111111</v>
+            <v>43917.209629629629</v>
           </cell>
           <cell r="M31" t="str">
-            <v>PROOSGMM_BDM_valida_recla</v>
+            <v>PROOSGMM_recla_LMP_NRLTCMP0</v>
           </cell>
           <cell r="P31" t="str">
             <v>Ended OK</v>
@@ -779,16 +787,16 @@
         </row>
         <row r="32">
           <cell r="A32" t="str">
-            <v>7497</v>
+            <v>56942</v>
           </cell>
           <cell r="E32">
-            <v>43913.18986111111</v>
+            <v>43917.193773148145</v>
           </cell>
           <cell r="I32">
-            <v>43913.210833333331</v>
+            <v>43917.21261574074</v>
           </cell>
           <cell r="M32" t="str">
-            <v>PROOSGMM_recla_LMP_NRLTRCL0</v>
+            <v>PROOSGMM_recla_LMP_NRLTDDC0</v>
           </cell>
           <cell r="P32" t="str">
             <v>Ended OK</v>
@@ -796,16 +804,16 @@
         </row>
         <row r="33">
           <cell r="A33" t="str">
-            <v>7484</v>
+            <v>21090</v>
           </cell>
           <cell r="E33">
-            <v>43913.18986111111</v>
+            <v>43917.167164351849</v>
           </cell>
           <cell r="I33">
-            <v>43913.212962962964</v>
+            <v>43917.214861111112</v>
           </cell>
           <cell r="M33" t="str">
-            <v>PROOSGMM_recla_LMP_NRLTCMP0</v>
+            <v>PROOSGMM_CNM_COBERT_DATOS_ADICIONALES</v>
           </cell>
           <cell r="P33" t="str">
             <v>Ended OK</v>
@@ -813,16 +821,16 @@
         </row>
         <row r="34">
           <cell r="A34" t="str">
-            <v>7486</v>
+            <v>16762</v>
           </cell>
           <cell r="E34">
-            <v>43913.18986111111</v>
+            <v>43917.134976851848</v>
           </cell>
           <cell r="I34">
-            <v>43913.215497685182</v>
+            <v>43917.215995370374</v>
           </cell>
           <cell r="M34" t="str">
-            <v>PROOSGMM_recla_LMP_NRLTDDC0</v>
+            <v>PROOSEOT_extevo_EOT_251</v>
           </cell>
           <cell r="P34" t="str">
             <v>Ended OK</v>
@@ -830,13 +838,13 @@
         </row>
         <row r="35">
           <cell r="A35" t="str">
-            <v>7490</v>
+            <v>56934</v>
           </cell>
           <cell r="E35">
-            <v>43913.18986111111</v>
+            <v>43917.193773148145</v>
           </cell>
           <cell r="I35">
-            <v>43913.219236111108</v>
+            <v>43917.216435185182</v>
           </cell>
           <cell r="M35" t="str">
             <v>PROOSGMM_recla_LMP_NRLTAAN0</v>
@@ -847,13 +855,13 @@
         </row>
         <row r="36">
           <cell r="A36" t="str">
-            <v>7485</v>
+            <v>56933</v>
           </cell>
           <cell r="E36">
-            <v>43913.18986111111</v>
+            <v>43917.193773148145</v>
           </cell>
           <cell r="I36">
-            <v>43913.232175925928</v>
+            <v>43917.228113425925</v>
           </cell>
           <cell r="M36" t="str">
             <v>PROOSGMM_recla_LMP_NRLTASP0</v>
@@ -864,13 +872,13 @@
         </row>
         <row r="37">
           <cell r="A37" t="str">
-            <v>7499</v>
+            <v>56939</v>
           </cell>
           <cell r="E37">
-            <v>43913.18986111111</v>
+            <v>43917.193773148145</v>
           </cell>
           <cell r="I37">
-            <v>43913.234594907408</v>
+            <v>43917.23060185185</v>
           </cell>
           <cell r="M37" t="str">
             <v>PROOSGMM_recla_LMP_NRLTSLR0</v>
@@ -881,16 +889,16 @@
         </row>
         <row r="38">
           <cell r="A38" t="str">
-            <v>16422</v>
+            <v>12960</v>
           </cell>
           <cell r="E38">
-            <v>43913.191076388888</v>
+            <v>43917.228125000001</v>
           </cell>
           <cell r="I38">
-            <v>43913.232893518521</v>
+            <v>43917.239305555559</v>
           </cell>
           <cell r="M38" t="str">
-            <v>PROOSGMM_CNM_ASEG_DATOS_ADICIONALES</v>
+            <v>PROOSGMM_CNM_RECLAMACION</v>
           </cell>
           <cell r="P38" t="str">
             <v>Ended OK</v>
@@ -898,16 +906,16 @@
         </row>
         <row r="39">
           <cell r="A39" t="str">
-            <v>2022</v>
+            <v>28850</v>
           </cell>
           <cell r="E39">
-            <v>43913.232187499998</v>
+            <v>43917.171273148146</v>
           </cell>
           <cell r="I39">
-            <v>43913.250335648147</v>
+            <v>43917.243888888886</v>
           </cell>
           <cell r="M39" t="str">
-            <v>PROOSGMM_CNM_RECLAMACION</v>
+            <v>PROOSEOT_extevo_EOT_351</v>
           </cell>
           <cell r="P39" t="str">
             <v>Ended OK</v>
@@ -915,16 +923,16 @@
         </row>
         <row r="40">
           <cell r="A40" t="str">
-            <v>38379</v>
+            <v>29295</v>
           </cell>
           <cell r="E40">
-            <v>43913.232638888891</v>
+            <v>43917.230613425927</v>
           </cell>
           <cell r="I40">
-            <v>43913.275520833333</v>
+            <v>43917.247094907405</v>
           </cell>
           <cell r="M40" t="str">
-            <v>PROOSGMM_orecla_LMP</v>
+            <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_GC</v>
           </cell>
           <cell r="P40" t="str">
             <v>Ended OK</v>
@@ -932,16 +940,16 @@
         </row>
         <row r="41">
           <cell r="A41" t="str">
-            <v>2625</v>
+            <v>5925</v>
           </cell>
           <cell r="E41">
-            <v>43913.232893518521</v>
+            <v>43917.214872685188</v>
           </cell>
           <cell r="I41">
-            <v>43913.276145833333</v>
+            <v>43917.257199074076</v>
           </cell>
           <cell r="M41" t="str">
-            <v>PROOSGMM_CNM_COBERT_DATOS_ADICIONALES</v>
+            <v>PROOSGMM_CNM_POLIZA_DATOS_ADICIONALES</v>
           </cell>
           <cell r="P41" t="str">
             <v>Ended OK</v>
@@ -949,16 +957,16 @@
         </row>
         <row r="42">
           <cell r="A42" t="str">
-            <v>40749</v>
+            <v>29293</v>
           </cell>
           <cell r="E42">
-            <v>43913.234606481485</v>
+            <v>43917.230613425927</v>
           </cell>
           <cell r="I42">
-            <v>43913.256099537037</v>
+            <v>43917.264467592591</v>
           </cell>
           <cell r="M42" t="str">
-            <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_GC</v>
+            <v>PROOSGMM_ENR_SOLICITUD_DG</v>
           </cell>
           <cell r="P42" t="str">
             <v>Ended OK</v>
@@ -966,16 +974,16 @@
         </row>
         <row r="43">
           <cell r="A43" t="str">
-            <v>40747</v>
+            <v>30739</v>
           </cell>
           <cell r="E43">
-            <v>43913.234606481485</v>
+            <v>43917.232638888891</v>
           </cell>
           <cell r="I43">
-            <v>43913.276087962964</v>
+            <v>43917.264918981484</v>
           </cell>
           <cell r="M43" t="str">
-            <v>PROOSGMM_ENR_SOLICITUD_DG</v>
+            <v>PROOSGMM_orecla_LMP</v>
           </cell>
           <cell r="P43" t="str">
             <v>Ended OK</v>
@@ -983,13 +991,13 @@
         </row>
         <row r="44">
           <cell r="A44" t="str">
-            <v>40748</v>
+            <v>29294</v>
           </cell>
           <cell r="E44">
-            <v>43913.234606481485</v>
+            <v>43917.230613425927</v>
           </cell>
           <cell r="I44">
-            <v>43913.295173611114</v>
+            <v>43917.274131944447</v>
           </cell>
           <cell r="M44" t="str">
             <v>PROOSGMM_ENR_SOLICITUD</v>
@@ -1000,47 +1008,47 @@
         </row>
         <row r="45">
           <cell r="A45" t="str">
-            <v>40760</v>
+            <v>25809</v>
           </cell>
           <cell r="E45">
-            <v>43913.234606481485</v>
+            <v>43917.145833333336</v>
           </cell>
           <cell r="I45">
-            <v>43913.316030092596</v>
+            <v>43917.282534722224</v>
           </cell>
           <cell r="M45" t="str">
-            <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_DG</v>
+            <v>PROOSGMM_oinfo_GMM_02</v>
           </cell>
           <cell r="P45" t="str">
-            <v>Ended OK</v>
+            <v>Ended Not OK</v>
           </cell>
         </row>
         <row r="46">
           <cell r="A46" t="str">
-            <v>8032</v>
+            <v>22365</v>
           </cell>
           <cell r="E46">
-            <v>43913.263888888891</v>
+            <v>43917.274131944447</v>
           </cell>
           <cell r="I46">
-            <v>43913.34002314815</v>
+            <v>43917.286747685182</v>
           </cell>
           <cell r="M46" t="str">
-            <v>PROOSGMM_oinfo_GMM_03</v>
+            <v>PROOSGMM_CNM_PADECIMIENTO</v>
           </cell>
           <cell r="P46" t="str">
-            <v>Ended Not OK</v>
+            <v>Ended OK</v>
           </cell>
         </row>
         <row r="47">
           <cell r="A47" t="str">
-            <v>8371</v>
+            <v>16633</v>
           </cell>
           <cell r="E47">
-            <v>43913.27553240741</v>
+            <v>43917.264930555553</v>
           </cell>
           <cell r="I47">
-            <v>43913.297060185185</v>
+            <v>43917.286851851852</v>
           </cell>
           <cell r="M47" t="str">
             <v>PROOSGMM_CNM_RECLAMACION_ACUMULADO</v>
@@ -1051,16 +1059,16 @@
         </row>
         <row r="48">
           <cell r="A48" t="str">
-            <v>8986</v>
+            <v>9591</v>
           </cell>
           <cell r="E48">
-            <v>43913.276145833333</v>
+            <v>43917.28125</v>
           </cell>
           <cell r="I48">
-            <v>43913.298668981479</v>
+            <v>43917.289317129631</v>
           </cell>
           <cell r="M48" t="str">
-            <v>PROOSGMM_CNM_POLIZA_DATOS_ADICIONALES</v>
+            <v>PROOSGMM_orecla_01</v>
           </cell>
           <cell r="P48" t="str">
             <v>Ended OK</v>
@@ -1068,16 +1076,16 @@
         </row>
         <row r="49">
           <cell r="A49" t="str">
-            <v>16130</v>
+            <v>22364</v>
           </cell>
           <cell r="E49">
-            <v>43913.28125</v>
+            <v>43917.274131944447</v>
           </cell>
           <cell r="I49">
-            <v>43913.287604166668</v>
+            <v>43917.290833333333</v>
           </cell>
           <cell r="M49" t="str">
-            <v>PROOSGMM_orecla_01</v>
+            <v>PROOSGMM_CNM_NOTAS_MEDICAS</v>
           </cell>
           <cell r="P49" t="str">
             <v>Ended OK</v>
@@ -1085,16 +1093,16 @@
         </row>
         <row r="50">
           <cell r="A50" t="str">
-            <v>17215</v>
+            <v>29300</v>
           </cell>
           <cell r="E50">
-            <v>43913.287615740737</v>
+            <v>43917.230613425927</v>
           </cell>
           <cell r="I50">
-            <v>43913.311180555553</v>
+            <v>43917.309918981482</v>
           </cell>
           <cell r="M50" t="str">
-            <v>PROOSGMM_CNM_COMPROBANTE</v>
+            <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_DG</v>
           </cell>
           <cell r="P50" t="str">
             <v>Ended OK</v>
@@ -1102,16 +1110,16 @@
         </row>
         <row r="51">
           <cell r="A51" t="str">
-            <v>22878</v>
+            <v>29410</v>
           </cell>
           <cell r="E51">
-            <v>43913.295185185183</v>
+            <v>43917.289317129631</v>
           </cell>
           <cell r="I51">
-            <v>43913.307789351849</v>
+            <v>43917.314166666663</v>
           </cell>
           <cell r="M51" t="str">
-            <v>PROOSGMM_CNM_PADECIMIENTO</v>
+            <v>PROOSGMM_CNM_COMPROBANTE</v>
           </cell>
           <cell r="P51" t="str">
             <v>Ended OK</v>
@@ -1119,16 +1127,16 @@
         </row>
         <row r="52">
           <cell r="A52" t="str">
-            <v>22877</v>
+            <v>22363</v>
           </cell>
           <cell r="E52">
-            <v>43913.295185185183</v>
+            <v>43917.274131944447</v>
           </cell>
           <cell r="I52">
-            <v>43913.311932870369</v>
+            <v>43917.318912037037</v>
           </cell>
           <cell r="M52" t="str">
-            <v>PROOSGMM_CNM_NOTAS_MEDICAS</v>
+            <v>PROOSGMM_CNM_SOLICITUD</v>
           </cell>
           <cell r="P52" t="str">
             <v>Ended OK</v>
@@ -1136,16 +1144,16 @@
         </row>
         <row r="53">
           <cell r="A53" t="str">
-            <v>22879</v>
+            <v>19250</v>
           </cell>
           <cell r="E53">
-            <v>43913.295185185183</v>
+            <v>43917.318923611114</v>
           </cell>
           <cell r="I53">
-            <v>43913.319062499999</v>
+            <v>43917.324525462966</v>
           </cell>
           <cell r="M53" t="str">
-            <v>PROOSGMM_CNM_SOLICITUD</v>
+            <v>PROOSGMM_FYF_wkf_gmm_fyf_gd</v>
           </cell>
           <cell r="P53" t="str">
             <v>Ended OK</v>
@@ -1153,16 +1161,16 @@
         </row>
         <row r="54">
           <cell r="A54" t="str">
-            <v>29978</v>
+            <v>562</v>
           </cell>
           <cell r="E54">
-            <v>43913.319074074076</v>
+            <v>43917.263888888891</v>
           </cell>
           <cell r="I54">
-            <v>43913.324745370373</v>
+            <v>43917.325127314813</v>
           </cell>
           <cell r="M54" t="str">
-            <v>PROOSGMM_FYF_wkf_gmm_fyf_gd</v>
+            <v>PROOSGMM_oinfo_GMM_03</v>
           </cell>
           <cell r="P54" t="str">
             <v>Ended OK</v>
@@ -1170,13 +1178,13 @@
         </row>
         <row r="55">
           <cell r="A55" t="str">
-            <v>6553</v>
+            <v>25959</v>
           </cell>
           <cell r="E55">
-            <v>43913.324756944443</v>
+            <v>43917.324537037035</v>
           </cell>
           <cell r="I55">
-            <v>43913.326145833336</v>
+            <v>43917.326006944444</v>
           </cell>
           <cell r="M55" t="str">
             <v>PROOSGMM_FYF_bq_fugasfraudesgmma</v>
@@ -1187,13 +1195,13 @@
         </row>
         <row r="56">
           <cell r="A56" t="str">
-            <v>11260</v>
+            <v>31052</v>
           </cell>
           <cell r="E56">
-            <v>43913.326157407406</v>
+            <v>43917.326006944444</v>
           </cell>
           <cell r="I56">
-            <v>43913.336562500001</v>
+            <v>43917.336180555554</v>
           </cell>
           <cell r="M56" t="str">
             <v>PROOSGMM_FYF_sh_bq_fugasyfraudes</v>
@@ -1505,21 +1513,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DBE8FFA-39E3-4C76-A19E-70A580C87EF3}">
-  <dimension ref="A1:F52"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="2" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="58.44140625" customWidth="1"/>
+    <col min="6" max="6" width="20.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1539,87 +1547,87 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>[1]Sheet1!A6</f>
-        <v>4700</v>
+        <v>40298</v>
       </c>
       <c r="B2" s="3">
         <f>[1]Sheet1!E6</f>
-        <v>43913.003472222219</v>
+        <v>43917.003472222219</v>
       </c>
       <c r="C2" s="3">
         <f>[1]Sheet1!I6</f>
-        <v>43913.006030092591</v>
+        <v>43917.039525462962</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" t="str">
         <f>[1]Sheet1!M6</f>
-        <v>PROOSGMM_oinfo_FYF_02</v>
+        <v>PROOSGMM_oinfo_FYF_01</v>
       </c>
       <c r="F2" t="str">
         <f>[1]Sheet1!P6</f>
-        <v>Ended Not OK</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>Ended OK</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>[1]Sheet1!A7</f>
-        <v>4705</v>
+        <v>40299</v>
       </c>
       <c r="B3" s="3">
         <f>[1]Sheet1!E7</f>
-        <v>43913.003472222219</v>
+        <v>43917.003472222219</v>
       </c>
       <c r="C3" s="3">
         <f>[1]Sheet1!I7</f>
-        <v>43913.011481481481</v>
+        <v>43917.05537037037</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" t="str">
         <f>[1]Sheet1!M7</f>
-        <v>PROOSGMM_oinfo_FYF_04</v>
+        <v>PROOSGMM_oinfo_FYF_02</v>
       </c>
       <c r="F3" t="str">
         <f>[1]Sheet1!P7</f>
-        <v>Ended Not OK</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>Ended OK</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>[1]Sheet1!A8</f>
-        <v>4699</v>
+        <v>40304</v>
       </c>
       <c r="B4" s="3">
         <f>[1]Sheet1!E8</f>
-        <v>43913.003472222219</v>
+        <v>43917.003472222219</v>
       </c>
       <c r="C4" s="3">
         <f>[1]Sheet1!I8</f>
-        <v>43913.018564814818</v>
+        <v>43917.05878472222</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" t="str">
         <f>[1]Sheet1!M8</f>
-        <v>PROOSGMM_oinfo_FYF_01</v>
+        <v>PROOSGMM_oinfo_FYF_04</v>
       </c>
       <c r="F4" t="str">
         <f>[1]Sheet1!P8</f>
-        <v>Ended Not OK</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>Ended OK</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>[1]Sheet1!A9</f>
-        <v>4706</v>
+        <v>40300</v>
       </c>
       <c r="B5" s="3">
         <f>[1]Sheet1!E9</f>
-        <v>43913.003472222219</v>
+        <v>43917.003472222219</v>
       </c>
       <c r="C5" s="3">
         <f>[1]Sheet1!I9</f>
-        <v>43913.037002314813</v>
+        <v>43917.062048611115</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" t="str">
@@ -1628,21 +1636,21 @@
       </c>
       <c r="F5" t="str">
         <f>[1]Sheet1!P9</f>
-        <v>Ended Not OK</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>Ended OK</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>[1]Sheet1!A10</f>
-        <v>4701</v>
+        <v>40306</v>
       </c>
       <c r="B6" s="3">
         <f>[1]Sheet1!E10</f>
-        <v>43913.003472222219</v>
+        <v>43917.003472222219</v>
       </c>
       <c r="C6" s="3">
         <f>[1]Sheet1!I10</f>
-        <v>43913.061215277776</v>
+        <v>43917.075277777774</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" t="str">
@@ -1651,21 +1659,21 @@
       </c>
       <c r="F6" t="str">
         <f>[1]Sheet1!P10</f>
-        <v>Ended Not OK</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>Ended OK</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>[1]Sheet1!A11</f>
-        <v>10014</v>
+        <v>44089</v>
       </c>
       <c r="B7" s="3">
         <f>[1]Sheet1!E11</f>
-        <v>43913.006944444445</v>
+        <v>43917.006944444445</v>
       </c>
       <c r="C7" s="3">
         <f>[1]Sheet1!I11</f>
-        <v>43913.070925925924</v>
+        <v>43917.080370370371</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" t="str">
@@ -1674,182 +1682,182 @@
       </c>
       <c r="F7" t="str">
         <f>[1]Sheet1!P11</f>
-        <v>Ended Not OK</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>Ended OK</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>[1]Sheet1!A12</f>
-        <v>57093</v>
+        <v>28966</v>
       </c>
       <c r="B8" s="3">
         <f>[1]Sheet1!E12</f>
-        <v>43913.072916666664</v>
+        <v>43917.058796296296</v>
       </c>
       <c r="C8" s="3">
         <f>[1]Sheet1!I12</f>
-        <v>43913.136157407411</v>
+        <v>43917.085358796299</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" t="str">
         <f>[1]Sheet1!M12</f>
-        <v>PROOSGMM_oinfo_GMM_01</v>
+        <v>PROOSGMM_wkf_gmm_taller_producto</v>
       </c>
       <c r="F8" t="str">
         <f>[1]Sheet1!P12</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>[1]Sheet1!A13</f>
-        <v>9694</v>
+        <v>39255</v>
       </c>
       <c r="B9" s="3">
         <f>[1]Sheet1!E13</f>
-        <v>43913.083333333336</v>
+        <v>43917.075289351851</v>
       </c>
       <c r="C9" s="3">
         <f>[1]Sheet1!I13</f>
-        <v>43913.128287037034</v>
+        <v>43917.096817129626</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" t="str">
         <f>[1]Sheet1!M13</f>
-        <v>PROOSGMM_oinfo_GMM_04</v>
+        <v>PROOSGMM_CNM_PROVEEDOR_MEDICO</v>
       </c>
       <c r="F9" t="str">
         <f>[1]Sheet1!P13</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>[1]Sheet1!A14</f>
-        <v>24352</v>
+        <v>4468</v>
       </c>
       <c r="B10" s="3">
         <f>[1]Sheet1!E14</f>
-        <v>43913.097222222219</v>
+        <v>43917.111111111109</v>
       </c>
       <c r="C10" s="3">
         <f>[1]Sheet1!I14</f>
-        <v>43913.147534722222</v>
+        <v>43917.117361111108</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" t="str">
         <f>[1]Sheet1!M14</f>
-        <v>PROOSEOT_extevo_EOT_101</v>
+        <v>PROOSGMM_oinfo_GMM_06</v>
       </c>
       <c r="F10" t="str">
         <f>[1]Sheet1!P14</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f>[1]Sheet1!A15</f>
-        <v>24353</v>
+        <v>28901</v>
       </c>
       <c r="B11" s="3">
         <f>[1]Sheet1!E15</f>
-        <v>43913.097222222219</v>
+        <v>43917.119444444441</v>
       </c>
       <c r="C11" s="3">
         <f>[1]Sheet1!I15</f>
-        <v>43913.186620370368</v>
+        <v>43917.12228009259</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" t="str">
         <f>[1]Sheet1!M15</f>
-        <v>PROOSEOT_extevo_EOT_301</v>
+        <v>PROOSCRM_wkf_cat_padecimiento_icd9</v>
       </c>
       <c r="F11" t="str">
         <f>[1]Sheet1!P15</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f>[1]Sheet1!A16</f>
-        <v>37411</v>
+        <v>29999</v>
       </c>
       <c r="B12" s="3">
         <f>[1]Sheet1!E16</f>
-        <v>43913.111111111109</v>
+        <v>43917.120138888888</v>
       </c>
       <c r="C12" s="3">
         <f>[1]Sheet1!I16</f>
-        <v>43913.1171875</v>
+        <v>43917.122974537036</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" t="str">
         <f>[1]Sheet1!M16</f>
-        <v>PROOSGMM_oinfo_GMM_06</v>
+        <v>PROOSCRM_wkf_cat_region_corporal</v>
       </c>
       <c r="F12" t="str">
         <f>[1]Sheet1!P16</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>[1]Sheet1!A17</f>
-        <v>13190</v>
+        <v>37232</v>
       </c>
       <c r="B13" s="3">
         <f>[1]Sheet1!E17</f>
-        <v>43913.119444444441</v>
+        <v>43917.072916666664</v>
       </c>
       <c r="C13" s="3">
         <f>[1]Sheet1!I17</f>
-        <v>43913.12228009259</v>
+        <v>43917.124016203707</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" t="str">
         <f>[1]Sheet1!M17</f>
-        <v>PROOSCRM_wkf_cat_padecimiento_icd9</v>
+        <v>PROOSGMM_oinfo_GMM_01</v>
       </c>
       <c r="F13" t="str">
         <f>[1]Sheet1!P17</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>[1]Sheet1!A18</f>
-        <v>13957</v>
+        <v>44370</v>
       </c>
       <c r="B14" s="3">
         <f>[1]Sheet1!E18</f>
-        <v>43913.120138888888</v>
+        <v>43917.083333333336</v>
       </c>
       <c r="C14" s="3">
         <f>[1]Sheet1!I18</f>
-        <v>43913.122974537036</v>
+        <v>43917.124432870369</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" t="str">
         <f>[1]Sheet1!M18</f>
-        <v>PROOSCRM_wkf_cat_region_corporal</v>
+        <v>PROOSGMM_oinfo_GMM_04</v>
       </c>
       <c r="F14" t="str">
         <f>[1]Sheet1!P18</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>[1]Sheet1!A19</f>
-        <v>19759</v>
+        <v>3315</v>
       </c>
       <c r="B15" s="3">
         <f>[1]Sheet1!E19</f>
-        <v>43913.125694444447</v>
+        <v>43917.125694444447</v>
       </c>
       <c r="C15" s="3">
         <f>[1]Sheet1!I19</f>
-        <v>43913.128530092596</v>
+        <v>43917.128530092596</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" t="str">
@@ -1861,18 +1869,18 @@
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>[1]Sheet1!A20</f>
-        <v>20795</v>
+        <v>4083</v>
       </c>
       <c r="B16" s="3">
         <f>[1]Sheet1!E20</f>
-        <v>43913.126388888886</v>
+        <v>43917.126388888886</v>
       </c>
       <c r="C16" s="3">
         <f>[1]Sheet1!I20</f>
-        <v>43913.129224537035</v>
+        <v>43917.129224537035</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" t="str">
@@ -1884,340 +1892,340 @@
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>[1]Sheet1!A21</f>
-        <v>30422</v>
+        <v>26978</v>
       </c>
       <c r="B17" s="3">
         <f>[1]Sheet1!E21</f>
-        <v>43913.136562500003</v>
+        <v>43917.116932870369</v>
       </c>
       <c r="C17" s="3">
         <f>[1]Sheet1!I21</f>
-        <v>43913.178472222222</v>
+        <v>43917.132303240738</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" t="str">
         <f>[1]Sheet1!M21</f>
-        <v>PROOSGMM_wkf_gmm_taller_producto</v>
+        <v>PROOSGMM_CNM_POLIZA</v>
       </c>
       <c r="F17" t="str">
         <f>[1]Sheet1!P21</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>[1]Sheet1!A22</f>
-        <v>11590</v>
+        <v>12774</v>
       </c>
       <c r="B18" s="3">
         <f>[1]Sheet1!E22</f>
-        <v>43913.137326388889</v>
+        <v>43917.097222222219</v>
       </c>
       <c r="C18" s="3">
         <f>[1]Sheet1!I22</f>
-        <v>43913.161597222221</v>
+        <v>43917.134965277779</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" t="str">
         <f>[1]Sheet1!M22</f>
-        <v>PROOSGMM_CNM_PROVEEDOR_MEDICO</v>
+        <v>PROOSEOT_extevo_EOT_101</v>
       </c>
       <c r="F18" t="str">
         <f>[1]Sheet1!P22</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>[1]Sheet1!A23</f>
-        <v>18113</v>
+        <v>9849</v>
       </c>
       <c r="B19" s="3">
         <f>[1]Sheet1!E23</f>
-        <v>43913.145833333336</v>
+        <v>43917.132303240738</v>
       </c>
       <c r="C19" s="3">
         <f>[1]Sheet1!I23</f>
-        <v>43913.224699074075</v>
+        <v>43917.167164351849</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" t="str">
         <f>[1]Sheet1!M23</f>
-        <v>PROOSGMM_oinfo_GMM_02</v>
+        <v>PROOSGMM_CNM_ASEG_DATOS_ADICIONALES</v>
       </c>
       <c r="F19" t="str">
         <f>[1]Sheet1!P23</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>[1]Sheet1!A24</f>
-        <v>13099</v>
+        <v>12775</v>
       </c>
       <c r="B20" s="3">
         <f>[1]Sheet1!E24</f>
-        <v>43913.147546296299</v>
+        <v>43917.097222222219</v>
       </c>
       <c r="C20" s="3">
         <f>[1]Sheet1!I24</f>
-        <v>43913.229953703703</v>
+        <v>43917.171261574076</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" t="str">
         <f>[1]Sheet1!M24</f>
-        <v>PROOSEOT_extevo_EOT_251</v>
+        <v>PROOSEOT_extevo_EOT_301</v>
       </c>
       <c r="F20" t="str">
         <f>[1]Sheet1!P24</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>[1]Sheet1!A25</f>
-        <v>16328</v>
+        <v>19529</v>
       </c>
       <c r="B21" s="3">
         <f>[1]Sheet1!E25</f>
-        <v>43913.166666666664</v>
+        <v>43917.166666666664</v>
       </c>
       <c r="C21" s="3">
         <f>[1]Sheet1!I25</f>
-        <v>43913.172291666669</v>
+        <v>43917.175081018519</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" t="str">
         <f>[1]Sheet1!M25</f>
-        <v>PROOSGMM_AZUL_wkf_gfvtagt0</v>
+        <v>PROOSGMM_AZUL_wkf_gccticdc</v>
       </c>
       <c r="F21" t="str">
         <f>[1]Sheet1!P25</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>[1]Sheet1!A26</f>
-        <v>16331</v>
+        <v>19559</v>
       </c>
       <c r="B22" s="3">
         <f>[1]Sheet1!E26</f>
-        <v>43913.166666666664</v>
+        <v>43917.166666666664</v>
       </c>
       <c r="C22" s="3">
         <f>[1]Sheet1!I26</f>
-        <v>43913.172291666669</v>
+        <v>43917.176481481481</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" t="str">
         <f>[1]Sheet1!M26</f>
-        <v>PROOSGMM_AZUL_wkf_gfvtcna0</v>
+        <v>PROOSGMM_AZUL_wkf_gfvtagt0</v>
       </c>
       <c r="F22" t="str">
         <f>[1]Sheet1!P26</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>[1]Sheet1!A27</f>
-        <v>16330</v>
+        <v>19581</v>
       </c>
       <c r="B23" s="3">
         <f>[1]Sheet1!E27</f>
-        <v>43913.166666666664</v>
+        <v>43917.166666666664</v>
       </c>
       <c r="C23" s="3">
         <f>[1]Sheet1!I27</f>
-        <v>43913.172291666669</v>
+        <v>43917.176481481481</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" t="str">
         <f>[1]Sheet1!M27</f>
-        <v>PROOSGMM_AZUL_wkf_gfvtfla0</v>
+        <v>PROOSGMM_AZUL_wkf_gfvtcna0</v>
       </c>
       <c r="F23" t="str">
         <f>[1]Sheet1!P27</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>[1]Sheet1!A28</f>
-        <v>16329</v>
+        <v>19558</v>
       </c>
       <c r="B24" s="3">
         <f>[1]Sheet1!E28</f>
-        <v>43913.166666666664</v>
+        <v>43917.166666666664</v>
       </c>
       <c r="C24" s="3">
         <f>[1]Sheet1!I28</f>
-        <v>43913.172291666669</v>
+        <v>43917.179270833331</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="str">
         <f>[1]Sheet1!M28</f>
-        <v>PROOSGMM_AZUL_wkf_gccticdc</v>
+        <v>PROOSGMM_AZUL_wkf_gfvtfla0</v>
       </c>
       <c r="F24" t="str">
         <f>[1]Sheet1!P28</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>[1]Sheet1!A29</f>
-        <v>1431</v>
+        <v>53798</v>
       </c>
       <c r="B25" s="3">
         <f>[1]Sheet1!E29</f>
-        <v>43913.178483796299</v>
+        <v>43917.191111111111</v>
       </c>
       <c r="C25" s="3">
         <f>[1]Sheet1!I29</f>
-        <v>43913.191064814811</v>
+        <v>43917.193773148145</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" t="str">
         <f>[1]Sheet1!M29</f>
-        <v>PROOSGMM_CNM_POLIZA</v>
+        <v>PROOSGMM_BDM_valida_recla</v>
       </c>
       <c r="F25" t="str">
         <f>[1]Sheet1!P29</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>[1]Sheet1!A30</f>
-        <v>8781</v>
+        <v>56945</v>
       </c>
       <c r="B26" s="3">
         <f>[1]Sheet1!E30</f>
-        <v>43913.186631944445</v>
+        <v>43917.193773148145</v>
       </c>
       <c r="C26" s="3">
         <f>[1]Sheet1!I30</f>
-        <v>43913.273206018515</v>
+        <v>43917.20952546296</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" t="str">
         <f>[1]Sheet1!M30</f>
-        <v>PROOSEOT_extevo_EOT_351</v>
+        <v>PROOSGMM_recla_LMP_NRLTRCL0</v>
       </c>
       <c r="F26" t="str">
         <f>[1]Sheet1!P30</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>[1]Sheet1!A31</f>
-        <v>3203</v>
+        <v>56935</v>
       </c>
       <c r="B27" s="3">
         <f>[1]Sheet1!E31</f>
-        <v>43913.1875</v>
+        <v>43917.193773148145</v>
       </c>
       <c r="C27" s="3">
         <f>[1]Sheet1!I31</f>
-        <v>43913.18986111111</v>
+        <v>43917.209629629629</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" t="str">
         <f>[1]Sheet1!M31</f>
-        <v>PROOSGMM_BDM_valida_recla</v>
+        <v>PROOSGMM_recla_LMP_NRLTCMP0</v>
       </c>
       <c r="F27" t="str">
         <f>[1]Sheet1!P31</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>[1]Sheet1!A32</f>
-        <v>7497</v>
+        <v>56942</v>
       </c>
       <c r="B28" s="3">
         <f>[1]Sheet1!E32</f>
-        <v>43913.18986111111</v>
+        <v>43917.193773148145</v>
       </c>
       <c r="C28" s="3">
         <f>[1]Sheet1!I32</f>
-        <v>43913.210833333331</v>
+        <v>43917.21261574074</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" t="str">
         <f>[1]Sheet1!M32</f>
-        <v>PROOSGMM_recla_LMP_NRLTRCL0</v>
+        <v>PROOSGMM_recla_LMP_NRLTDDC0</v>
       </c>
       <c r="F28" t="str">
         <f>[1]Sheet1!P32</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>[1]Sheet1!A33</f>
-        <v>7484</v>
+        <v>21090</v>
       </c>
       <c r="B29" s="3">
         <f>[1]Sheet1!E33</f>
-        <v>43913.18986111111</v>
+        <v>43917.167164351849</v>
       </c>
       <c r="C29" s="3">
         <f>[1]Sheet1!I33</f>
-        <v>43913.212962962964</v>
+        <v>43917.214861111112</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" t="str">
         <f>[1]Sheet1!M33</f>
-        <v>PROOSGMM_recla_LMP_NRLTCMP0</v>
+        <v>PROOSGMM_CNM_COBERT_DATOS_ADICIONALES</v>
       </c>
       <c r="F29" t="str">
         <f>[1]Sheet1!P33</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="str">
         <f>[1]Sheet1!A34</f>
-        <v>7486</v>
+        <v>16762</v>
       </c>
       <c r="B30" s="3">
         <f>[1]Sheet1!E34</f>
-        <v>43913.18986111111</v>
+        <v>43917.134976851848</v>
       </c>
       <c r="C30" s="3">
         <f>[1]Sheet1!I34</f>
-        <v>43913.215497685182</v>
+        <v>43917.215995370374</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" t="str">
         <f>[1]Sheet1!M34</f>
-        <v>PROOSGMM_recla_LMP_NRLTDDC0</v>
+        <v>PROOSEOT_extevo_EOT_251</v>
       </c>
       <c r="F30" t="str">
         <f>[1]Sheet1!P34</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="str">
         <f>[1]Sheet1!A35</f>
-        <v>7490</v>
+        <v>56934</v>
       </c>
       <c r="B31" s="3">
         <f>[1]Sheet1!E35</f>
-        <v>43913.18986111111</v>
+        <v>43917.193773148145</v>
       </c>
       <c r="C31" s="3">
         <f>[1]Sheet1!I35</f>
-        <v>43913.219236111108</v>
+        <v>43917.216435185182</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" t="str">
@@ -2229,18 +2237,18 @@
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="str">
         <f>[1]Sheet1!A36</f>
-        <v>7485</v>
+        <v>56933</v>
       </c>
       <c r="B32" s="3">
         <f>[1]Sheet1!E36</f>
-        <v>43913.18986111111</v>
+        <v>43917.193773148145</v>
       </c>
       <c r="C32" s="3">
         <f>[1]Sheet1!I36</f>
-        <v>43913.232175925928</v>
+        <v>43917.228113425925</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" t="str">
@@ -2252,18 +2260,18 @@
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="str">
         <f>[1]Sheet1!A37</f>
-        <v>7499</v>
+        <v>56939</v>
       </c>
       <c r="B33" s="3">
         <f>[1]Sheet1!E37</f>
-        <v>43913.18986111111</v>
+        <v>43917.193773148145</v>
       </c>
       <c r="C33" s="3">
         <f>[1]Sheet1!I37</f>
-        <v>43913.234594907408</v>
+        <v>43917.23060185185</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" t="str">
@@ -2275,156 +2283,156 @@
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="str">
         <f>[1]Sheet1!A38</f>
-        <v>16422</v>
+        <v>12960</v>
       </c>
       <c r="B34" s="3">
         <f>[1]Sheet1!E38</f>
-        <v>43913.191076388888</v>
+        <v>43917.228125000001</v>
       </c>
       <c r="C34" s="3">
         <f>[1]Sheet1!I38</f>
-        <v>43913.232893518521</v>
+        <v>43917.239305555559</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" t="str">
         <f>[1]Sheet1!M38</f>
-        <v>PROOSGMM_CNM_ASEG_DATOS_ADICIONALES</v>
+        <v>PROOSGMM_CNM_RECLAMACION</v>
       </c>
       <c r="F34" t="str">
         <f>[1]Sheet1!P38</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="str">
         <f>[1]Sheet1!A39</f>
-        <v>2022</v>
+        <v>28850</v>
       </c>
       <c r="B35" s="3">
         <f>[1]Sheet1!E39</f>
-        <v>43913.232187499998</v>
+        <v>43917.171273148146</v>
       </c>
       <c r="C35" s="3">
         <f>[1]Sheet1!I39</f>
-        <v>43913.250335648147</v>
+        <v>43917.243888888886</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" t="str">
         <f>[1]Sheet1!M39</f>
-        <v>PROOSGMM_CNM_RECLAMACION</v>
+        <v>PROOSEOT_extevo_EOT_351</v>
       </c>
       <c r="F35" t="str">
         <f>[1]Sheet1!P39</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>[1]Sheet1!A40</f>
-        <v>38379</v>
+        <v>29295</v>
       </c>
       <c r="B36" s="3">
         <f>[1]Sheet1!E40</f>
-        <v>43913.232638888891</v>
+        <v>43917.230613425927</v>
       </c>
       <c r="C36" s="3">
         <f>[1]Sheet1!I40</f>
-        <v>43913.275520833333</v>
+        <v>43917.247094907405</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" t="str">
         <f>[1]Sheet1!M40</f>
-        <v>PROOSGMM_orecla_LMP</v>
+        <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_GC</v>
       </c>
       <c r="F36" t="str">
         <f>[1]Sheet1!P40</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>[1]Sheet1!A41</f>
-        <v>2625</v>
+        <v>5925</v>
       </c>
       <c r="B37" s="3">
         <f>[1]Sheet1!E41</f>
-        <v>43913.232893518521</v>
+        <v>43917.214872685188</v>
       </c>
       <c r="C37" s="3">
         <f>[1]Sheet1!I41</f>
-        <v>43913.276145833333</v>
+        <v>43917.257199074076</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" t="str">
         <f>[1]Sheet1!M41</f>
-        <v>PROOSGMM_CNM_COBERT_DATOS_ADICIONALES</v>
+        <v>PROOSGMM_CNM_POLIZA_DATOS_ADICIONALES</v>
       </c>
       <c r="F37" t="str">
         <f>[1]Sheet1!P41</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="str">
         <f>[1]Sheet1!A42</f>
-        <v>40749</v>
+        <v>29293</v>
       </c>
       <c r="B38" s="3">
         <f>[1]Sheet1!E42</f>
-        <v>43913.234606481485</v>
+        <v>43917.230613425927</v>
       </c>
       <c r="C38" s="3">
         <f>[1]Sheet1!I42</f>
-        <v>43913.256099537037</v>
+        <v>43917.264467592591</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" t="str">
         <f>[1]Sheet1!M42</f>
-        <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_GC</v>
+        <v>PROOSGMM_ENR_SOLICITUD_DG</v>
       </c>
       <c r="F38" t="str">
         <f>[1]Sheet1!P42</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>[1]Sheet1!A43</f>
-        <v>40747</v>
+        <v>30739</v>
       </c>
       <c r="B39" s="3">
         <f>[1]Sheet1!E43</f>
-        <v>43913.234606481485</v>
+        <v>43917.232638888891</v>
       </c>
       <c r="C39" s="3">
         <f>[1]Sheet1!I43</f>
-        <v>43913.276087962964</v>
+        <v>43917.264918981484</v>
       </c>
       <c r="D39" s="3"/>
       <c r="E39" t="str">
         <f>[1]Sheet1!M43</f>
-        <v>PROOSGMM_ENR_SOLICITUD_DG</v>
+        <v>PROOSGMM_orecla_LMP</v>
       </c>
       <c r="F39" t="str">
         <f>[1]Sheet1!P43</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="str">
         <f>[1]Sheet1!A44</f>
-        <v>40748</v>
+        <v>29294</v>
       </c>
       <c r="B40" s="3">
         <f>[1]Sheet1!E44</f>
-        <v>43913.234606481485</v>
+        <v>43917.230613425927</v>
       </c>
       <c r="C40" s="3">
         <f>[1]Sheet1!I44</f>
-        <v>43913.295173611114</v>
+        <v>43917.274131944447</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" t="str">
@@ -2436,64 +2444,64 @@
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="str">
         <f>[1]Sheet1!A45</f>
-        <v>40760</v>
+        <v>25809</v>
       </c>
       <c r="B41" s="3">
         <f>[1]Sheet1!E45</f>
-        <v>43913.234606481485</v>
+        <v>43917.145833333336</v>
       </c>
       <c r="C41" s="3">
         <f>[1]Sheet1!I45</f>
-        <v>43913.316030092596</v>
+        <v>43917.282534722224</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" t="str">
         <f>[1]Sheet1!M45</f>
-        <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_DG</v>
+        <v>PROOSGMM_oinfo_GMM_02</v>
       </c>
       <c r="F41" t="str">
         <f>[1]Sheet1!P45</f>
-        <v>Ended OK</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>Ended Not OK</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f>[1]Sheet1!A46</f>
-        <v>8032</v>
+        <v>22365</v>
       </c>
       <c r="B42" s="3">
         <f>[1]Sheet1!E46</f>
-        <v>43913.263888888891</v>
+        <v>43917.274131944447</v>
       </c>
       <c r="C42" s="3">
         <f>[1]Sheet1!I46</f>
-        <v>43913.34002314815</v>
+        <v>43917.286747685182</v>
       </c>
       <c r="D42" s="3"/>
       <c r="E42" t="str">
         <f>[1]Sheet1!M46</f>
-        <v>PROOSGMM_oinfo_GMM_03</v>
+        <v>PROOSGMM_CNM_PADECIMIENTO</v>
       </c>
       <c r="F42" t="str">
         <f>[1]Sheet1!P46</f>
-        <v>Ended Not OK</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>Ended OK</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f>[1]Sheet1!A47</f>
-        <v>8371</v>
+        <v>16633</v>
       </c>
       <c r="B43" s="3">
         <f>[1]Sheet1!E47</f>
-        <v>43913.27553240741</v>
+        <v>43917.264930555553</v>
       </c>
       <c r="C43" s="3">
         <f>[1]Sheet1!I47</f>
-        <v>43913.297060185185</v>
+        <v>43917.286851851852</v>
       </c>
       <c r="D43" s="3"/>
       <c r="E43" t="str">
@@ -2505,179 +2513,179 @@
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="str">
         <f>[1]Sheet1!A48</f>
-        <v>8986</v>
+        <v>9591</v>
       </c>
       <c r="B44" s="3">
         <f>[1]Sheet1!E48</f>
-        <v>43913.276145833333</v>
+        <v>43917.28125</v>
       </c>
       <c r="C44" s="3">
         <f>[1]Sheet1!I48</f>
-        <v>43913.298668981479</v>
+        <v>43917.289317129631</v>
       </c>
       <c r="D44" s="3"/>
       <c r="E44" t="str">
         <f>[1]Sheet1!M48</f>
-        <v>PROOSGMM_CNM_POLIZA_DATOS_ADICIONALES</v>
+        <v>PROOSGMM_orecla_01</v>
       </c>
       <c r="F44" t="str">
         <f>[1]Sheet1!P48</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="str">
         <f>[1]Sheet1!A49</f>
-        <v>16130</v>
+        <v>22364</v>
       </c>
       <c r="B45" s="3">
         <f>[1]Sheet1!E49</f>
-        <v>43913.28125</v>
+        <v>43917.274131944447</v>
       </c>
       <c r="C45" s="3">
         <f>[1]Sheet1!I49</f>
-        <v>43913.287604166668</v>
+        <v>43917.290833333333</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" t="str">
         <f>[1]Sheet1!M49</f>
-        <v>PROOSGMM_orecla_01</v>
+        <v>PROOSGMM_CNM_NOTAS_MEDICAS</v>
       </c>
       <c r="F45" t="str">
         <f>[1]Sheet1!P49</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="str">
         <f>[1]Sheet1!A50</f>
-        <v>17215</v>
+        <v>29300</v>
       </c>
       <c r="B46" s="3">
         <f>[1]Sheet1!E50</f>
-        <v>43913.287615740737</v>
+        <v>43917.230613425927</v>
       </c>
       <c r="C46" s="3">
         <f>[1]Sheet1!I50</f>
-        <v>43913.311180555553</v>
+        <v>43917.309918981482</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" t="str">
         <f>[1]Sheet1!M50</f>
-        <v>PROOSGMM_CNM_COMPROBANTE</v>
+        <v>PROOSGMM_CNM_CARTAS_AUTORIZACION_DG</v>
       </c>
       <c r="F46" t="str">
         <f>[1]Sheet1!P50</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="str">
         <f>[1]Sheet1!A51</f>
-        <v>22878</v>
+        <v>29410</v>
       </c>
       <c r="B47" s="3">
         <f>[1]Sheet1!E51</f>
-        <v>43913.295185185183</v>
+        <v>43917.289317129631</v>
       </c>
       <c r="C47" s="3">
         <f>[1]Sheet1!I51</f>
-        <v>43913.307789351849</v>
+        <v>43917.314166666663</v>
       </c>
       <c r="D47" s="3"/>
       <c r="E47" t="str">
         <f>[1]Sheet1!M51</f>
-        <v>PROOSGMM_CNM_PADECIMIENTO</v>
+        <v>PROOSGMM_CNM_COMPROBANTE</v>
       </c>
       <c r="F47" t="str">
         <f>[1]Sheet1!P51</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="str">
         <f>[1]Sheet1!A52</f>
-        <v>22877</v>
+        <v>22363</v>
       </c>
       <c r="B48" s="3">
         <f>[1]Sheet1!E52</f>
-        <v>43913.295185185183</v>
+        <v>43917.274131944447</v>
       </c>
       <c r="C48" s="3">
         <f>[1]Sheet1!I52</f>
-        <v>43913.311932870369</v>
+        <v>43917.318912037037</v>
       </c>
       <c r="D48" s="3"/>
       <c r="E48" t="str">
         <f>[1]Sheet1!M52</f>
-        <v>PROOSGMM_CNM_NOTAS_MEDICAS</v>
+        <v>PROOSGMM_CNM_SOLICITUD</v>
       </c>
       <c r="F48" t="str">
         <f>[1]Sheet1!P52</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="str">
         <f>[1]Sheet1!A53</f>
-        <v>22879</v>
+        <v>19250</v>
       </c>
       <c r="B49" s="3">
         <f>[1]Sheet1!E53</f>
-        <v>43913.295185185183</v>
+        <v>43917.318923611114</v>
       </c>
       <c r="C49" s="3">
         <f>[1]Sheet1!I53</f>
-        <v>43913.319062499999</v>
+        <v>43917.324525462966</v>
       </c>
       <c r="D49" s="3"/>
       <c r="E49" t="str">
         <f>[1]Sheet1!M53</f>
-        <v>PROOSGMM_CNM_SOLICITUD</v>
+        <v>PROOSGMM_FYF_wkf_gmm_fyf_gd</v>
       </c>
       <c r="F49" t="str">
         <f>[1]Sheet1!P53</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="str">
         <f>[1]Sheet1!A54</f>
-        <v>29978</v>
+        <v>562</v>
       </c>
       <c r="B50" s="3">
         <f>[1]Sheet1!E54</f>
-        <v>43913.319074074076</v>
+        <v>43917.263888888891</v>
       </c>
       <c r="C50" s="3">
         <f>[1]Sheet1!I54</f>
-        <v>43913.324745370373</v>
+        <v>43917.325127314813</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" t="str">
         <f>[1]Sheet1!M54</f>
-        <v>PROOSGMM_FYF_wkf_gmm_fyf_gd</v>
+        <v>PROOSGMM_oinfo_GMM_03</v>
       </c>
       <c r="F50" t="str">
         <f>[1]Sheet1!P54</f>
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="str">
         <f>[1]Sheet1!A55</f>
-        <v>6553</v>
+        <v>25959</v>
       </c>
       <c r="B51" s="3">
         <f>[1]Sheet1!E55</f>
-        <v>43913.324756944443</v>
+        <v>43917.324537037035</v>
       </c>
       <c r="C51" s="3">
         <f>[1]Sheet1!I55</f>
-        <v>43913.326145833336</v>
+        <v>43917.326006944444</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" t="str">
@@ -2689,18 +2697,18 @@
         <v>Ended OK</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="str">
         <f>[1]Sheet1!A56</f>
-        <v>11260</v>
+        <v>31052</v>
       </c>
       <c r="B52" s="3">
         <f>[1]Sheet1!E56</f>
-        <v>43913.326157407406</v>
+        <v>43917.326006944444</v>
       </c>
       <c r="C52" s="3">
         <f>[1]Sheet1!I56</f>
-        <v>43913.336562500001</v>
+        <v>43917.336180555554</v>
       </c>
       <c r="D52" s="3"/>
       <c r="E52" t="str">
@@ -2711,6 +2719,11 @@
         <f>[1]Sheet1!P56</f>
         <v>Ended OK</v>
       </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2726,265 +2739,265 @@
       <selection activeCell="F2" sqref="F2:F52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F2" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F3" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F5" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F7" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F8" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F9" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F10" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F11" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F12" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F13" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F14" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F15" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F16" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F17" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" ht="72" x14ac:dyDescent="0.3">
       <c r="F18" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F19" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F20" s="4" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F21" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F22" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:6" ht="72" x14ac:dyDescent="0.3">
       <c r="F23" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F24" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F25" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="6:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F26" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F27" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F28" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F29" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F30" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F31" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F32" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F33" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F34" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F35" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F36" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F37" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F38" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F39" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F40" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F41" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="42" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F42" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F43" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="F44" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="6:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F45" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="46" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F46" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F47" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F48" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="49" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F49" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="50" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F50" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="F51" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="6:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="F52" s="5" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="F2:F53">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F2:F53">
     <sortCondition ref="F1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>